<commit_message>
Mercado laboral y Titulos
</commit_message>
<xml_diff>
--- a/Data/Construcciones.xlsx
+++ b/Data/Construcciones.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HP\Documents\Estudio\proyecto camara de comercio-20210502T212657Z-001\proyecto camara de comercio\dashboards\Graficas R y Python\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E782C2A8-8914-4B5C-96FE-D38F26298CA1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B78AA6C-6697-4A57-98ED-6F711A330E5B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="2" activeTab="7" xr2:uid="{0BCF3411-F03E-4660-8BC8-E5D33D9799DE}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="2" activeTab="6" xr2:uid="{0BCF3411-F03E-4660-8BC8-E5D33D9799DE}"/>
   </bookViews>
   <sheets>
     <sheet name="Area_censada" sheetId="1" r:id="rId1"/>
@@ -19,14 +19,15 @@
     <sheet name="Vivi_new_o_IVPN" sheetId="3" r:id="rId4"/>
     <sheet name="Vis_no" sheetId="8" r:id="rId5"/>
     <sheet name="Area_proc_destino" sheetId="4" r:id="rId6"/>
-    <sheet name="vivienda" sheetId="5" r:id="rId7"/>
-    <sheet name="destinos" sheetId="7" r:id="rId8"/>
-    <sheet name="guia" sheetId="6" r:id="rId9"/>
-    <sheet name="guia_1" sheetId="10" r:id="rId10"/>
+    <sheet name="In Costos" sheetId="11" r:id="rId7"/>
+    <sheet name="vivienda" sheetId="5" r:id="rId8"/>
+    <sheet name="destinos" sheetId="7" r:id="rId9"/>
+    <sheet name="guia" sheetId="6" r:id="rId10"/>
+    <sheet name="guia_1" sheetId="10" r:id="rId11"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="7" hidden="1">destinos!$A$1:$H$952</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="6" hidden="1">vivienda!$A$1:$I$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="8" hidden="1">destinos!$A$1:$H$952</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="7" hidden="1">vivienda!$A$1:$I$1</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -47,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12531" uniqueCount="339">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12597" uniqueCount="382">
   <si>
     <t>IV</t>
   </si>
@@ -1108,6 +1109,135 @@
   <si>
     <t>est</t>
   </si>
+  <si>
+    <t>Índice de Costos de la Construcción de Vivienda  - ICCV</t>
+  </si>
+  <si>
+    <t>A2. ICCV - Variación mensual y anual total ICCV, por tipos de vivienda según ciudades</t>
+  </si>
+  <si>
+    <t>Enero 2021</t>
+  </si>
+  <si>
+    <t>Ciudades</t>
+  </si>
+  <si>
+    <t>Total nacional</t>
+  </si>
+  <si>
+    <t>Vivienda unifamiliar</t>
+  </si>
+  <si>
+    <t>Vivienda multifamiliar</t>
+  </si>
+  <si>
+    <t>Mensual</t>
+  </si>
+  <si>
+    <t>Anual</t>
+  </si>
+  <si>
+    <t>Nacional</t>
+  </si>
+  <si>
+    <t>Medellín</t>
+  </si>
+  <si>
+    <t>Barranquilla</t>
+  </si>
+  <si>
+    <t>Bogotá, D.C.</t>
+  </si>
+  <si>
+    <t>Cartagena</t>
+  </si>
+  <si>
+    <t>Manizales</t>
+  </si>
+  <si>
+    <t>Popayán</t>
+  </si>
+  <si>
+    <t>Neiva</t>
+  </si>
+  <si>
+    <t>Santa Marta</t>
+  </si>
+  <si>
+    <t>Pasto</t>
+  </si>
+  <si>
+    <t>Cúcuta</t>
+  </si>
+  <si>
+    <t>Armenia</t>
+  </si>
+  <si>
+    <t>Pereira</t>
+  </si>
+  <si>
+    <t>Bucaramanga</t>
+  </si>
+  <si>
+    <t>Ibagué</t>
+  </si>
+  <si>
+    <t>Cali</t>
+  </si>
+  <si>
+    <t>A5. ICCV -  Variación mensual, año corrido y anual, total ICCV (2017 - 2021)</t>
+  </si>
+  <si>
+    <t>Meses</t>
+  </si>
+  <si>
+    <t>Año corrido</t>
+  </si>
+  <si>
+    <t>Enero</t>
+  </si>
+  <si>
+    <t>Febrero</t>
+  </si>
+  <si>
+    <t>Marzo</t>
+  </si>
+  <si>
+    <t>Abril</t>
+  </si>
+  <si>
+    <t>Mayo</t>
+  </si>
+  <si>
+    <t>Junio</t>
+  </si>
+  <si>
+    <t>Julio</t>
+  </si>
+  <si>
+    <t>Agosto</t>
+  </si>
+  <si>
+    <t>Septiembre</t>
+  </si>
+  <si>
+    <t>Octubre</t>
+  </si>
+  <si>
+    <t>Noviembre</t>
+  </si>
+  <si>
+    <t>Diciembre</t>
+  </si>
+  <si>
+    <t>A1. ICCV - Variación mensual y anual, total ICCV y por tipos de vivienda</t>
+  </si>
+  <si>
+    <t>Enero 2010-2021</t>
+  </si>
+  <si>
+    <t>Años</t>
+  </si>
 </sst>
 </file>
 
@@ -1119,7 +1249,7 @@
     <numFmt numFmtId="166" formatCode="0.0"/>
     <numFmt numFmtId="167" formatCode="_-* #,##0.00\ [$€]_-;\-* #,##0.00\ [$€]_-;_-* &quot;-&quot;??\ [$€]_-;_-@_-"/>
   </numFmts>
-  <fonts count="33" x14ac:knownFonts="1">
+  <fonts count="35" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1347,8 +1477,21 @@
       <name val="Segoe UI"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color rgb="FF0000FF"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="40">
+  <fills count="41">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1568,8 +1711,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-4.9989318521683403E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="18">
+  <borders count="25">
     <border>
       <left/>
       <right/>
@@ -1768,8 +1917,89 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="70">
+  <cellStyleXfs count="72">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
@@ -1843,8 +2073,10 @@
     <xf numFmtId="0" fontId="15" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="15" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="15" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="18" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="68">
+  <cellXfs count="144">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="17" fillId="34" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
@@ -2011,8 +2243,234 @@
     <xf numFmtId="0" fontId="28" fillId="36" borderId="0" xfId="37" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="20" xfId="34" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="36" borderId="0" xfId="34" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="36" borderId="15" xfId="34" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="39" borderId="18" xfId="34" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="39" borderId="0" xfId="34" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="39" borderId="15" xfId="34" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="12" xfId="34" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="20" xfId="34" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="25" fillId="36" borderId="19" xfId="34" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="25" fillId="36" borderId="14" xfId="34" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="25" fillId="36" borderId="17" xfId="34" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="23" xfId="34" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="12" xfId="34" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="22" fillId="36" borderId="0" xfId="71" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="22" fillId="36" borderId="18" xfId="71" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="22" fillId="35" borderId="18" xfId="71" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="25" fillId="40" borderId="14" xfId="34" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="20" xfId="34" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="21" xfId="34" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="25" fillId="0" borderId="15" xfId="34" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="2" fontId="25" fillId="0" borderId="0" xfId="71" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="25" fillId="0" borderId="16" xfId="71" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="25" fillId="0" borderId="18" xfId="71" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="22" fillId="36" borderId="15" xfId="34" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="166" fontId="22" fillId="0" borderId="15" xfId="34" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="2" fontId="22" fillId="0" borderId="0" xfId="71" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="22" fillId="0" borderId="18" xfId="71" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="22" fillId="36" borderId="17" xfId="34" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="2" fontId="22" fillId="36" borderId="14" xfId="71" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="22" fillId="36" borderId="19" xfId="71" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="12" xfId="34" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="36" borderId="18" xfId="34" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="24" xfId="34" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="20" xfId="34" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="21" xfId="34" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="24" xfId="34" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="21" xfId="34" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="36" borderId="14" xfId="34" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="36" borderId="17" xfId="34" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="22" fillId="36" borderId="0" xfId="71" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="21" xfId="34" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="25" fillId="0" borderId="0" xfId="71" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="25" fillId="0" borderId="16" xfId="71" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="22" fillId="0" borderId="0" xfId="71" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="22" fillId="36" borderId="14" xfId="71" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="35" borderId="14" xfId="34" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="21" xfId="34" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="35" borderId="14" xfId="34" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="22" fillId="0" borderId="0" xfId="71" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="2" fontId="22" fillId="0" borderId="16" xfId="71" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="22" fillId="36" borderId="0" xfId="71" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="2" fontId="22" fillId="36" borderId="14" xfId="71" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="35" borderId="20" xfId="34" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="25" fillId="36" borderId="14" xfId="71" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="35" borderId="12" xfId="34" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="35" borderId="20" xfId="34" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="35" borderId="22" xfId="34" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="35" borderId="16" xfId="34" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="35" borderId="12" xfId="34" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="36" borderId="19" xfId="34" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="22" fillId="36" borderId="0" xfId="71" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="22" fillId="35" borderId="0" xfId="71" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="40" borderId="14" xfId="34" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="25" fillId="36" borderId="14" xfId="71" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="40" borderId="20" xfId="34" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="40" borderId="20" xfId="34" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="34" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="36" borderId="0" xfId="34" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="22" fillId="36" borderId="0" xfId="34" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="22" fillId="0" borderId="0" xfId="34" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="35" borderId="0" xfId="34" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="36" borderId="14" xfId="34" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="35" borderId="21" xfId="34" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="22" fillId="35" borderId="18" xfId="34" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="22" fillId="36" borderId="18" xfId="34" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="25" fillId="36" borderId="19" xfId="34" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="70">
+  <cellStyles count="72">
     <cellStyle name="20% - Accent1" xfId="17" builtinId="30" customBuiltin="1"/>
     <cellStyle name="20% - Accent2" xfId="20" builtinId="34" customBuiltin="1"/>
     <cellStyle name="20% - Accent3" xfId="23" builtinId="38" customBuiltin="1"/>
@@ -2057,6 +2515,7 @@
     <cellStyle name="Heading 3" xfId="3" builtinId="18" customBuiltin="1"/>
     <cellStyle name="Heading 4" xfId="4" builtinId="19" customBuiltin="1"/>
     <cellStyle name="Hipervínculo 2" xfId="39" xr:uid="{BD9255CC-A171-4358-842E-797118BAA51D}"/>
+    <cellStyle name="Hipervínculo 2 2" xfId="70" xr:uid="{6D51A181-D52C-4496-9585-FB4C00E2A05D}"/>
     <cellStyle name="Input" xfId="7" builtinId="20" customBuiltin="1"/>
     <cellStyle name="Linked Cell" xfId="10" builtinId="24" customBuiltin="1"/>
     <cellStyle name="Millares 2" xfId="53" xr:uid="{565899C5-31D4-4434-AA70-09EC7037655A}"/>
@@ -2073,6 +2532,7 @@
     <cellStyle name="Notas 2" xfId="59" xr:uid="{6F3D9383-BED5-4B9D-BB59-CBEA3EAF22BC}"/>
     <cellStyle name="Note" xfId="13" builtinId="10" customBuiltin="1"/>
     <cellStyle name="Output" xfId="8" builtinId="21" customBuiltin="1"/>
+    <cellStyle name="Percent 2" xfId="71" xr:uid="{3493121C-03B7-42FD-9CBA-A6F7CB8CA5AA}"/>
     <cellStyle name="Porcentaje 2" xfId="36" xr:uid="{D0E28FC2-8A51-45A9-8132-770A634E0E21}"/>
     <cellStyle name="Porcentaje 2 2" xfId="60" xr:uid="{E5751E99-785C-498D-B5D2-7B8511B1D65C}"/>
     <cellStyle name="Porcentaje 3" xfId="61" xr:uid="{A3C73DAD-F9F0-40FA-AF93-7E184E2B3D8B}"/>
@@ -3244,6 +3704,690 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9F45B1B4-192A-4769-AF8C-9EA5A2391269}">
+  <dimension ref="A1:I49"/>
+  <sheetViews>
+    <sheetView topLeftCell="A32" workbookViewId="0">
+      <selection activeCell="C39" sqref="C39:C44"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1" s="34"/>
+      <c r="B1" s="34"/>
+      <c r="C1" s="34"/>
+      <c r="D1" s="34"/>
+      <c r="E1" s="34"/>
+      <c r="F1" s="34"/>
+      <c r="G1" s="34"/>
+      <c r="H1" s="34"/>
+      <c r="I1" s="34"/>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" s="34"/>
+      <c r="B2" s="34"/>
+      <c r="C2" s="34"/>
+      <c r="D2" s="34"/>
+      <c r="E2" s="34"/>
+      <c r="F2" s="34"/>
+      <c r="G2" s="34"/>
+      <c r="H2" s="34"/>
+      <c r="I2" s="34"/>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" s="62" t="s">
+        <v>49</v>
+      </c>
+      <c r="B3" s="63"/>
+      <c r="C3" s="63"/>
+      <c r="D3" s="63"/>
+      <c r="E3" s="63"/>
+      <c r="F3" s="63"/>
+      <c r="G3" s="63"/>
+      <c r="H3" s="63"/>
+      <c r="I3" s="63"/>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" s="64"/>
+      <c r="B4" s="65"/>
+      <c r="C4" s="65"/>
+      <c r="D4" s="65"/>
+      <c r="E4" s="65"/>
+      <c r="F4" s="65"/>
+      <c r="G4" s="65"/>
+      <c r="H4" s="65"/>
+      <c r="I4" s="65"/>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" s="66" t="s">
+        <v>50</v>
+      </c>
+      <c r="B5" s="66"/>
+      <c r="C5" s="66"/>
+      <c r="D5" s="66"/>
+      <c r="E5" s="66"/>
+      <c r="F5" s="66"/>
+      <c r="G5" s="66"/>
+      <c r="H5" s="66"/>
+      <c r="I5" s="66"/>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" s="67"/>
+      <c r="B6" s="67"/>
+      <c r="C6" s="67"/>
+      <c r="D6" s="67"/>
+      <c r="E6" s="67"/>
+      <c r="F6" s="67"/>
+      <c r="G6" s="67"/>
+      <c r="H6" s="67"/>
+      <c r="I6" s="67"/>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7" s="67"/>
+      <c r="B7" s="67"/>
+      <c r="C7" s="67"/>
+      <c r="D7" s="67"/>
+      <c r="E7" s="67"/>
+      <c r="F7" s="67"/>
+      <c r="G7" s="67"/>
+      <c r="H7" s="67"/>
+      <c r="I7" s="67"/>
+    </row>
+    <row r="8" spans="1:9" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A8" s="35"/>
+      <c r="B8" s="36"/>
+      <c r="C8" s="35"/>
+      <c r="D8" s="35"/>
+      <c r="E8" s="35"/>
+      <c r="F8" s="35"/>
+      <c r="G8" s="35"/>
+      <c r="H8" s="35"/>
+      <c r="I8" s="35"/>
+    </row>
+    <row r="9" spans="1:9" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A9" s="35"/>
+      <c r="B9" s="37" t="s">
+        <v>28</v>
+      </c>
+      <c r="C9" s="38"/>
+      <c r="D9" s="38"/>
+      <c r="E9" s="35"/>
+      <c r="F9" s="35"/>
+      <c r="G9" s="35"/>
+      <c r="H9" s="35"/>
+      <c r="I9" s="35"/>
+    </row>
+    <row r="10" spans="1:9" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A10" s="35"/>
+      <c r="B10" s="38" t="s">
+        <v>51</v>
+      </c>
+      <c r="C10" s="38"/>
+      <c r="D10" s="38"/>
+      <c r="E10" s="35"/>
+      <c r="F10" s="35"/>
+      <c r="G10" s="35"/>
+      <c r="H10" s="35"/>
+      <c r="I10" s="35"/>
+    </row>
+    <row r="11" spans="1:9" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A11" s="35"/>
+      <c r="B11" s="38"/>
+      <c r="C11" s="38"/>
+      <c r="D11" s="38"/>
+      <c r="E11" s="35"/>
+      <c r="F11" s="35"/>
+      <c r="G11" s="35"/>
+      <c r="H11" s="35"/>
+      <c r="I11" s="35"/>
+    </row>
+    <row r="12" spans="1:9" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A12" s="35"/>
+      <c r="B12" s="37" t="s">
+        <v>29</v>
+      </c>
+      <c r="C12" s="38"/>
+      <c r="D12" s="38"/>
+      <c r="E12" s="35"/>
+      <c r="F12" s="35"/>
+      <c r="G12" s="35"/>
+      <c r="H12" s="35"/>
+      <c r="I12" s="35"/>
+    </row>
+    <row r="13" spans="1:9" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A13" s="35"/>
+      <c r="B13" s="38" t="s">
+        <v>52</v>
+      </c>
+      <c r="C13" s="38"/>
+      <c r="D13" s="38"/>
+      <c r="E13" s="35"/>
+      <c r="F13" s="35"/>
+      <c r="G13" s="35"/>
+      <c r="H13" s="35"/>
+      <c r="I13" s="35"/>
+    </row>
+    <row r="14" spans="1:9" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A14" s="35"/>
+      <c r="B14" s="38"/>
+      <c r="C14" s="38"/>
+      <c r="D14" s="38"/>
+      <c r="E14" s="35"/>
+      <c r="F14" s="35"/>
+      <c r="G14" s="35"/>
+      <c r="H14" s="35"/>
+      <c r="I14" s="35"/>
+    </row>
+    <row r="15" spans="1:9" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A15" s="35"/>
+      <c r="B15" s="37" t="s">
+        <v>53</v>
+      </c>
+      <c r="C15" s="38"/>
+      <c r="D15" s="38"/>
+      <c r="E15" s="35"/>
+      <c r="F15" s="35"/>
+      <c r="G15" s="35"/>
+      <c r="H15" s="35"/>
+      <c r="I15" s="35"/>
+    </row>
+    <row r="16" spans="1:9" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A16" s="35"/>
+      <c r="B16" s="38">
+        <v>1</v>
+      </c>
+      <c r="C16" s="38" t="s">
+        <v>54</v>
+      </c>
+      <c r="D16" s="38"/>
+      <c r="E16" s="35"/>
+      <c r="F16" s="35"/>
+      <c r="G16" s="35"/>
+      <c r="H16" s="35"/>
+      <c r="I16" s="35"/>
+    </row>
+    <row r="17" spans="1:9" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A17" s="35"/>
+      <c r="B17" s="38">
+        <v>2</v>
+      </c>
+      <c r="C17" s="38" t="s">
+        <v>55</v>
+      </c>
+      <c r="D17" s="38"/>
+      <c r="E17" s="35"/>
+      <c r="F17" s="35"/>
+      <c r="G17" s="35"/>
+      <c r="H17" s="35"/>
+      <c r="I17" s="35"/>
+    </row>
+    <row r="18" spans="1:9" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A18" s="35"/>
+      <c r="B18" s="38">
+        <v>3</v>
+      </c>
+      <c r="C18" s="38" t="s">
+        <v>56</v>
+      </c>
+      <c r="D18" s="38"/>
+      <c r="E18" s="35"/>
+      <c r="F18" s="35"/>
+      <c r="G18" s="35"/>
+      <c r="H18" s="35"/>
+      <c r="I18" s="35"/>
+    </row>
+    <row r="19" spans="1:9" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A19" s="35"/>
+      <c r="B19" s="38">
+        <v>4</v>
+      </c>
+      <c r="C19" s="38" t="s">
+        <v>57</v>
+      </c>
+      <c r="D19" s="38"/>
+      <c r="E19" s="35"/>
+      <c r="F19" s="35"/>
+      <c r="G19" s="35"/>
+      <c r="H19" s="35"/>
+      <c r="I19" s="35"/>
+    </row>
+    <row r="20" spans="1:9" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A20" s="35"/>
+      <c r="B20" s="38">
+        <v>5</v>
+      </c>
+      <c r="C20" s="38" t="s">
+        <v>58</v>
+      </c>
+      <c r="D20" s="38"/>
+      <c r="E20" s="35"/>
+      <c r="F20" s="35"/>
+      <c r="G20" s="35"/>
+      <c r="H20" s="35"/>
+      <c r="I20" s="35"/>
+    </row>
+    <row r="21" spans="1:9" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A21" s="35"/>
+      <c r="B21" s="38">
+        <v>6</v>
+      </c>
+      <c r="C21" s="38" t="s">
+        <v>59</v>
+      </c>
+      <c r="D21" s="38"/>
+      <c r="E21" s="35"/>
+      <c r="F21" s="35"/>
+      <c r="G21" s="35"/>
+      <c r="H21" s="35"/>
+      <c r="I21" s="35"/>
+    </row>
+    <row r="22" spans="1:9" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A22" s="35"/>
+      <c r="B22" s="38">
+        <v>7</v>
+      </c>
+      <c r="C22" s="38" t="s">
+        <v>60</v>
+      </c>
+      <c r="D22" s="38"/>
+      <c r="E22" s="35"/>
+      <c r="F22" s="35"/>
+      <c r="G22" s="35"/>
+      <c r="H22" s="35"/>
+      <c r="I22" s="35"/>
+    </row>
+    <row r="23" spans="1:9" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A23" s="35"/>
+      <c r="B23" s="38">
+        <v>8</v>
+      </c>
+      <c r="C23" s="38" t="s">
+        <v>61</v>
+      </c>
+      <c r="D23" s="38"/>
+      <c r="E23" s="35"/>
+      <c r="F23" s="35"/>
+      <c r="G23" s="35"/>
+      <c r="H23" s="35"/>
+      <c r="I23" s="35"/>
+    </row>
+    <row r="24" spans="1:9" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A24" s="35"/>
+      <c r="B24" s="38">
+        <v>9</v>
+      </c>
+      <c r="C24" s="38" t="s">
+        <v>62</v>
+      </c>
+      <c r="D24" s="38"/>
+      <c r="E24" s="35"/>
+      <c r="F24" s="35"/>
+      <c r="G24" s="35"/>
+      <c r="H24" s="35"/>
+      <c r="I24" s="35"/>
+    </row>
+    <row r="25" spans="1:9" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A25" s="35"/>
+      <c r="B25" s="38">
+        <v>10</v>
+      </c>
+      <c r="C25" s="38" t="s">
+        <v>63</v>
+      </c>
+      <c r="D25" s="38"/>
+      <c r="E25" s="35"/>
+      <c r="F25" s="35"/>
+      <c r="G25" s="35"/>
+      <c r="H25" s="35"/>
+      <c r="I25" s="35"/>
+    </row>
+    <row r="26" spans="1:9" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A26" s="35"/>
+      <c r="B26" s="38">
+        <v>11</v>
+      </c>
+      <c r="C26" s="38" t="s">
+        <v>64</v>
+      </c>
+      <c r="D26" s="38"/>
+      <c r="E26" s="35"/>
+      <c r="F26" s="35"/>
+      <c r="G26" s="35"/>
+      <c r="H26" s="35"/>
+      <c r="I26" s="35"/>
+    </row>
+    <row r="27" spans="1:9" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A27" s="35"/>
+      <c r="B27" s="38">
+        <v>12</v>
+      </c>
+      <c r="C27" s="38" t="s">
+        <v>65</v>
+      </c>
+      <c r="D27" s="38"/>
+      <c r="E27" s="35"/>
+      <c r="F27" s="35"/>
+      <c r="G27" s="35"/>
+      <c r="H27" s="35"/>
+      <c r="I27" s="35"/>
+    </row>
+    <row r="28" spans="1:9" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A28" s="35"/>
+      <c r="B28" s="38"/>
+      <c r="C28" s="38"/>
+      <c r="D28" s="38"/>
+      <c r="E28" s="35"/>
+      <c r="F28" s="35"/>
+      <c r="G28" s="35"/>
+      <c r="H28" s="35"/>
+      <c r="I28" s="35"/>
+    </row>
+    <row r="29" spans="1:9" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A29" s="35"/>
+      <c r="B29" s="37" t="s">
+        <v>30</v>
+      </c>
+      <c r="C29" s="38"/>
+      <c r="D29" s="38"/>
+      <c r="E29" s="35"/>
+      <c r="F29" s="35"/>
+      <c r="G29" s="35"/>
+      <c r="H29" s="35"/>
+      <c r="I29" s="35"/>
+    </row>
+    <row r="30" spans="1:9" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A30" s="35"/>
+      <c r="B30" s="38">
+        <v>1</v>
+      </c>
+      <c r="C30" s="38" t="s">
+        <v>66</v>
+      </c>
+      <c r="D30" s="38"/>
+      <c r="E30" s="35"/>
+      <c r="F30" s="35"/>
+      <c r="G30" s="35"/>
+      <c r="H30" s="35"/>
+      <c r="I30" s="35"/>
+    </row>
+    <row r="31" spans="1:9" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A31" s="35"/>
+      <c r="B31" s="38">
+        <v>2</v>
+      </c>
+      <c r="C31" s="38" t="s">
+        <v>67</v>
+      </c>
+      <c r="D31" s="38"/>
+      <c r="E31" s="35"/>
+      <c r="F31" s="35"/>
+      <c r="G31" s="35"/>
+      <c r="H31" s="35"/>
+      <c r="I31" s="35"/>
+    </row>
+    <row r="32" spans="1:9" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A32" s="35"/>
+      <c r="B32" s="38"/>
+      <c r="C32" s="38"/>
+      <c r="D32" s="38"/>
+      <c r="E32" s="35"/>
+      <c r="F32" s="35"/>
+      <c r="G32" s="35"/>
+      <c r="H32" s="35"/>
+      <c r="I32" s="35"/>
+    </row>
+    <row r="33" spans="1:9" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A33" s="35"/>
+      <c r="B33" s="37" t="s">
+        <v>31</v>
+      </c>
+      <c r="C33" s="38"/>
+      <c r="D33" s="38"/>
+      <c r="E33" s="35"/>
+      <c r="F33" s="35"/>
+      <c r="G33" s="35"/>
+      <c r="H33" s="35"/>
+      <c r="I33" s="35"/>
+    </row>
+    <row r="34" spans="1:9" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A34" s="35"/>
+      <c r="B34" s="38">
+        <v>1</v>
+      </c>
+      <c r="C34" s="38" t="s">
+        <v>68</v>
+      </c>
+      <c r="D34" s="38"/>
+      <c r="E34" s="35"/>
+      <c r="F34" s="35"/>
+      <c r="G34" s="35"/>
+      <c r="H34" s="35"/>
+      <c r="I34" s="35"/>
+    </row>
+    <row r="35" spans="1:9" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A35" s="35"/>
+      <c r="B35" s="38">
+        <v>2</v>
+      </c>
+      <c r="C35" s="38" t="s">
+        <v>69</v>
+      </c>
+      <c r="D35" s="38"/>
+      <c r="E35" s="35"/>
+      <c r="F35" s="35"/>
+      <c r="G35" s="35"/>
+      <c r="H35" s="35"/>
+      <c r="I35" s="35"/>
+    </row>
+    <row r="36" spans="1:9" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A36" s="35"/>
+      <c r="B36" s="38">
+        <v>3</v>
+      </c>
+      <c r="C36" s="38" t="s">
+        <v>70</v>
+      </c>
+      <c r="D36" s="38"/>
+      <c r="E36" s="35"/>
+      <c r="F36" s="35"/>
+      <c r="G36" s="35"/>
+      <c r="H36" s="35"/>
+      <c r="I36" s="35"/>
+    </row>
+    <row r="37" spans="1:9" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A37" s="35"/>
+      <c r="B37" s="38"/>
+      <c r="C37" s="38"/>
+      <c r="D37" s="38"/>
+      <c r="E37" s="35"/>
+      <c r="F37" s="35"/>
+      <c r="G37" s="35"/>
+      <c r="H37" s="35"/>
+      <c r="I37" s="35"/>
+    </row>
+    <row r="38" spans="1:9" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A38" s="35"/>
+      <c r="B38" s="37" t="s">
+        <v>32</v>
+      </c>
+      <c r="C38" s="38"/>
+      <c r="D38" s="38"/>
+      <c r="E38" s="35"/>
+      <c r="F38" s="35"/>
+      <c r="G38" s="35"/>
+      <c r="H38" s="35"/>
+      <c r="I38" s="35"/>
+    </row>
+    <row r="39" spans="1:9" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A39" s="35"/>
+      <c r="B39" s="38">
+        <v>1</v>
+      </c>
+      <c r="C39" s="38" t="s">
+        <v>71</v>
+      </c>
+      <c r="D39" s="38"/>
+      <c r="E39" s="35"/>
+      <c r="F39" s="35"/>
+      <c r="G39" s="35"/>
+      <c r="H39" s="35"/>
+      <c r="I39" s="35"/>
+    </row>
+    <row r="40" spans="1:9" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A40" s="35"/>
+      <c r="B40" s="38">
+        <v>2</v>
+      </c>
+      <c r="C40" s="38" t="s">
+        <v>72</v>
+      </c>
+      <c r="D40" s="38"/>
+      <c r="E40" s="35"/>
+      <c r="F40" s="35"/>
+      <c r="G40" s="35"/>
+      <c r="H40" s="35"/>
+      <c r="I40" s="35"/>
+    </row>
+    <row r="41" spans="1:9" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A41" s="35"/>
+      <c r="B41" s="38">
+        <v>3</v>
+      </c>
+      <c r="C41" s="38" t="s">
+        <v>73</v>
+      </c>
+      <c r="D41" s="38"/>
+      <c r="E41" s="35"/>
+      <c r="F41" s="35"/>
+      <c r="G41" s="35"/>
+      <c r="H41" s="35"/>
+      <c r="I41" s="35"/>
+    </row>
+    <row r="42" spans="1:9" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A42" s="35"/>
+      <c r="B42" s="38">
+        <v>4</v>
+      </c>
+      <c r="C42" s="38" t="s">
+        <v>74</v>
+      </c>
+      <c r="D42" s="38"/>
+      <c r="E42" s="35"/>
+      <c r="F42" s="35"/>
+      <c r="G42" s="35"/>
+      <c r="H42" s="35"/>
+      <c r="I42" s="35"/>
+    </row>
+    <row r="43" spans="1:9" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A43" s="35"/>
+      <c r="B43" s="38">
+        <v>5</v>
+      </c>
+      <c r="C43" s="38" t="s">
+        <v>75</v>
+      </c>
+      <c r="D43" s="38"/>
+      <c r="E43" s="35"/>
+      <c r="F43" s="35"/>
+      <c r="G43" s="35"/>
+      <c r="H43" s="35"/>
+      <c r="I43" s="35"/>
+    </row>
+    <row r="44" spans="1:9" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A44" s="35"/>
+      <c r="B44" s="38">
+        <v>6</v>
+      </c>
+      <c r="C44" s="38" t="s">
+        <v>76</v>
+      </c>
+      <c r="D44" s="38"/>
+      <c r="E44" s="35"/>
+      <c r="F44" s="35"/>
+      <c r="G44" s="35"/>
+      <c r="H44" s="35"/>
+      <c r="I44" s="35"/>
+    </row>
+    <row r="45" spans="1:9" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A45" s="35"/>
+      <c r="B45" s="38"/>
+      <c r="C45" s="38"/>
+      <c r="D45" s="38"/>
+      <c r="E45" s="35"/>
+      <c r="F45" s="35"/>
+      <c r="G45" s="35"/>
+      <c r="H45" s="35"/>
+      <c r="I45" s="35"/>
+    </row>
+    <row r="46" spans="1:9" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A46" s="35"/>
+      <c r="B46" s="37" t="s">
+        <v>77</v>
+      </c>
+      <c r="C46" s="38"/>
+      <c r="D46" s="38"/>
+      <c r="E46" s="35"/>
+      <c r="F46" s="35"/>
+      <c r="G46" s="35"/>
+      <c r="H46" s="35"/>
+      <c r="I46" s="35"/>
+    </row>
+    <row r="47" spans="1:9" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A47" s="35"/>
+      <c r="B47" s="38">
+        <v>77</v>
+      </c>
+      <c r="C47" s="38" t="s">
+        <v>78</v>
+      </c>
+      <c r="D47" s="38"/>
+      <c r="E47" s="35"/>
+      <c r="F47" s="35"/>
+      <c r="G47" s="35"/>
+      <c r="H47" s="35"/>
+      <c r="I47" s="35"/>
+    </row>
+    <row r="48" spans="1:9" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A48" s="35"/>
+      <c r="B48" s="38">
+        <v>88</v>
+      </c>
+      <c r="C48" s="38" t="s">
+        <v>79</v>
+      </c>
+      <c r="D48" s="38"/>
+      <c r="E48" s="35"/>
+      <c r="F48" s="35"/>
+      <c r="G48" s="35"/>
+      <c r="H48" s="35"/>
+      <c r="I48" s="35"/>
+    </row>
+    <row r="49" spans="1:9" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A49" s="35"/>
+      <c r="B49" s="38">
+        <v>302</v>
+      </c>
+      <c r="C49" s="38" t="s">
+        <v>80</v>
+      </c>
+      <c r="D49" s="38"/>
+      <c r="E49" s="35"/>
+      <c r="F49" s="35"/>
+      <c r="G49" s="35"/>
+      <c r="H49" s="35"/>
+      <c r="I49" s="35"/>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A3:I4"/>
+    <mergeCell ref="A5:I7"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{32CD59C8-6E57-4D69-AED3-4801600C50C7}">
   <dimension ref="A1:E13"/>
   <sheetViews>
@@ -6620,12 +7764,6 @@
     </row>
   </sheetData>
   <mergeCells count="16">
-    <mergeCell ref="A12:A13"/>
-    <mergeCell ref="A2:A3"/>
-    <mergeCell ref="A4:A5"/>
-    <mergeCell ref="A6:A7"/>
-    <mergeCell ref="A8:A9"/>
-    <mergeCell ref="A10:A11"/>
     <mergeCell ref="A28:A29"/>
     <mergeCell ref="A30:A31"/>
     <mergeCell ref="A32:A33"/>
@@ -6636,6 +7774,12 @@
     <mergeCell ref="A20:A22"/>
     <mergeCell ref="A23:A25"/>
     <mergeCell ref="A26:A27"/>
+    <mergeCell ref="A12:A13"/>
+    <mergeCell ref="A2:A3"/>
+    <mergeCell ref="A4:A5"/>
+    <mergeCell ref="A6:A7"/>
+    <mergeCell ref="A8:A9"/>
+    <mergeCell ref="A10:A11"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -7626,11 +8770,1685 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{665B1F9E-B70E-40B2-9416-996EC19C363B}">
+  <dimension ref="A1:S40"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J7" sqref="J7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:19" ht="20.25" x14ac:dyDescent="0.25">
+      <c r="A1" s="73" t="s">
+        <v>339</v>
+      </c>
+      <c r="B1" s="72"/>
+      <c r="C1" s="72"/>
+      <c r="D1" s="72"/>
+      <c r="E1" s="72"/>
+      <c r="F1" s="72"/>
+      <c r="G1" s="72"/>
+      <c r="H1" s="72"/>
+      <c r="I1" s="71"/>
+      <c r="K1" s="73" t="s">
+        <v>339</v>
+      </c>
+      <c r="L1" s="72"/>
+      <c r="M1" s="72"/>
+      <c r="N1" s="72"/>
+      <c r="O1" s="72"/>
+      <c r="P1" s="72"/>
+      <c r="Q1" s="72"/>
+      <c r="R1" s="72"/>
+      <c r="S1" s="71"/>
+    </row>
+    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A2" s="70" t="s">
+        <v>340</v>
+      </c>
+      <c r="B2" s="69"/>
+      <c r="C2" s="69"/>
+      <c r="D2" s="69"/>
+      <c r="E2" s="69"/>
+      <c r="F2" s="69"/>
+      <c r="G2" s="69"/>
+      <c r="H2" s="69"/>
+      <c r="I2" s="99"/>
+      <c r="K2" s="70" t="s">
+        <v>379</v>
+      </c>
+      <c r="L2" s="69"/>
+      <c r="M2" s="69"/>
+      <c r="N2" s="69"/>
+      <c r="O2" s="69"/>
+      <c r="P2" s="69"/>
+      <c r="Q2" s="69"/>
+      <c r="R2" s="69"/>
+      <c r="S2" s="99"/>
+    </row>
+    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A3" s="78" t="s">
+        <v>341</v>
+      </c>
+      <c r="B3" s="77"/>
+      <c r="C3" s="77"/>
+      <c r="D3" s="77"/>
+      <c r="E3" s="77"/>
+      <c r="F3" s="77"/>
+      <c r="G3" s="77"/>
+      <c r="H3" s="77"/>
+      <c r="I3" s="76"/>
+      <c r="K3" s="106" t="s">
+        <v>380</v>
+      </c>
+      <c r="L3" s="105"/>
+      <c r="M3" s="105"/>
+      <c r="N3" s="105"/>
+      <c r="O3" s="105"/>
+      <c r="P3" s="105"/>
+      <c r="Q3" s="105"/>
+      <c r="R3" s="105"/>
+      <c r="S3" s="127"/>
+    </row>
+    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A4" s="84"/>
+      <c r="B4" s="84"/>
+      <c r="C4" s="84"/>
+      <c r="D4" s="84"/>
+      <c r="E4" s="84"/>
+      <c r="F4" s="84"/>
+      <c r="G4" s="84"/>
+      <c r="H4" s="84"/>
+      <c r="I4" s="84"/>
+      <c r="K4" s="130"/>
+      <c r="L4" s="130"/>
+      <c r="M4" s="130"/>
+      <c r="N4" s="130"/>
+      <c r="O4" s="130"/>
+      <c r="P4" s="130"/>
+      <c r="Q4" s="130"/>
+      <c r="R4" s="130"/>
+      <c r="S4" s="130"/>
+    </row>
+    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A5" s="98" t="s">
+        <v>342</v>
+      </c>
+      <c r="B5" s="75" t="s">
+        <v>343</v>
+      </c>
+      <c r="C5" s="75"/>
+      <c r="D5" s="74" t="s">
+        <v>344</v>
+      </c>
+      <c r="E5" s="74"/>
+      <c r="F5" s="68" t="s">
+        <v>345</v>
+      </c>
+      <c r="G5" s="68"/>
+      <c r="H5" s="80" t="s">
+        <v>82</v>
+      </c>
+      <c r="I5" s="79"/>
+      <c r="K5" s="140" t="s">
+        <v>381</v>
+      </c>
+      <c r="L5" s="122" t="s">
+        <v>343</v>
+      </c>
+      <c r="M5" s="122"/>
+      <c r="N5" s="123" t="s">
+        <v>344</v>
+      </c>
+      <c r="O5" s="123"/>
+      <c r="P5" s="126" t="s">
+        <v>345</v>
+      </c>
+      <c r="Q5" s="126"/>
+      <c r="R5" s="125" t="s">
+        <v>82</v>
+      </c>
+      <c r="S5" s="124"/>
+    </row>
+    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A6" s="86"/>
+      <c r="B6" s="85" t="s">
+        <v>346</v>
+      </c>
+      <c r="C6" s="85" t="s">
+        <v>347</v>
+      </c>
+      <c r="D6" s="85" t="s">
+        <v>346</v>
+      </c>
+      <c r="E6" s="85" t="s">
+        <v>347</v>
+      </c>
+      <c r="F6" s="85" t="s">
+        <v>346</v>
+      </c>
+      <c r="G6" s="85" t="s">
+        <v>347</v>
+      </c>
+      <c r="H6" s="85" t="s">
+        <v>346</v>
+      </c>
+      <c r="I6" s="85" t="s">
+        <v>347</v>
+      </c>
+      <c r="K6" s="133"/>
+      <c r="L6" s="132" t="s">
+        <v>346</v>
+      </c>
+      <c r="M6" s="132" t="s">
+        <v>347</v>
+      </c>
+      <c r="N6" s="132" t="s">
+        <v>346</v>
+      </c>
+      <c r="O6" s="132" t="s">
+        <v>347</v>
+      </c>
+      <c r="P6" s="132" t="s">
+        <v>346</v>
+      </c>
+      <c r="Q6" s="132" t="s">
+        <v>347</v>
+      </c>
+      <c r="R6" s="132" t="s">
+        <v>346</v>
+      </c>
+      <c r="S6" s="132" t="s">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A7" s="87" t="s">
+        <v>348</v>
+      </c>
+      <c r="B7" s="88">
+        <v>0.78150575</v>
+      </c>
+      <c r="C7" s="88">
+        <v>4.2904800099999996</v>
+      </c>
+      <c r="D7" s="89">
+        <v>0.80362663999999995</v>
+      </c>
+      <c r="E7" s="88">
+        <v>4.4415545400000003</v>
+      </c>
+      <c r="F7" s="89">
+        <v>0.76837789000000001</v>
+      </c>
+      <c r="G7" s="88">
+        <v>4.2008612699999999</v>
+      </c>
+      <c r="H7" s="88">
+        <v>0.86256116999999999</v>
+      </c>
+      <c r="I7" s="90">
+        <v>4.1818283300000001</v>
+      </c>
+      <c r="K7" s="134">
+        <v>2010</v>
+      </c>
+      <c r="L7" s="129">
+        <v>0.57897215999999996</v>
+      </c>
+      <c r="M7" s="129">
+        <v>-1.0573935699999999</v>
+      </c>
+      <c r="N7" s="129">
+        <v>0.68812176000000003</v>
+      </c>
+      <c r="O7" s="129">
+        <v>-0.24195717</v>
+      </c>
+      <c r="P7" s="129">
+        <v>0.51474140999999995</v>
+      </c>
+      <c r="Q7" s="129">
+        <v>-1.5327257700000001</v>
+      </c>
+      <c r="R7" s="129">
+        <v>0.71808844999999999</v>
+      </c>
+      <c r="S7" s="141">
+        <v>-0.45617882999999998</v>
+      </c>
+    </row>
+    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A8" s="91" t="s">
+        <v>349</v>
+      </c>
+      <c r="B8" s="81">
+        <v>0.53731563000000004</v>
+      </c>
+      <c r="C8" s="81">
+        <v>6.0146508399999998</v>
+      </c>
+      <c r="D8" s="81">
+        <v>0.48983014000000002</v>
+      </c>
+      <c r="E8" s="81">
+        <v>5.6858005199999999</v>
+      </c>
+      <c r="F8" s="81">
+        <v>0.55871903999999994</v>
+      </c>
+      <c r="G8" s="81">
+        <v>6.1634434200000001</v>
+      </c>
+      <c r="H8" s="81">
+        <v>0.57918488999999995</v>
+      </c>
+      <c r="I8" s="82">
+        <v>5.7860704700000003</v>
+      </c>
+      <c r="K8" s="135">
+        <v>2011</v>
+      </c>
+      <c r="L8" s="128">
+        <v>0.64548320999999997</v>
+      </c>
+      <c r="M8" s="128">
+        <v>1.8324376</v>
+      </c>
+      <c r="N8" s="128">
+        <v>0.71080597000000001</v>
+      </c>
+      <c r="O8" s="128">
+        <v>2.0132556899999998</v>
+      </c>
+      <c r="P8" s="128">
+        <v>0.60690376000000001</v>
+      </c>
+      <c r="Q8" s="128">
+        <v>1.7257182799999999</v>
+      </c>
+      <c r="R8" s="128">
+        <v>0.6499085</v>
+      </c>
+      <c r="S8" s="142">
+        <v>2.0591456699999999</v>
+      </c>
+    </row>
+    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A9" s="92" t="s">
+        <v>350</v>
+      </c>
+      <c r="B9" s="93">
+        <v>0.86292365999999998</v>
+      </c>
+      <c r="C9" s="93">
+        <v>5.7980360600000003</v>
+      </c>
+      <c r="D9" s="93">
+        <v>0.74383277999999997</v>
+      </c>
+      <c r="E9" s="93">
+        <v>5.8765013100000001</v>
+      </c>
+      <c r="F9" s="93">
+        <v>0.89733412999999995</v>
+      </c>
+      <c r="G9" s="93">
+        <v>5.7754200000000004</v>
+      </c>
+      <c r="H9" s="93">
+        <v>0.77324093000000005</v>
+      </c>
+      <c r="I9" s="94">
+        <v>5.9189964000000002</v>
+      </c>
+      <c r="K9" s="134">
+        <v>2012</v>
+      </c>
+      <c r="L9" s="129">
+        <v>0.95620645999999998</v>
+      </c>
+      <c r="M9" s="129">
+        <v>7.2011984699999996</v>
+      </c>
+      <c r="N9" s="129">
+        <v>1.0948603400000001</v>
+      </c>
+      <c r="O9" s="129">
+        <v>7.0307757500000001</v>
+      </c>
+      <c r="P9" s="129">
+        <v>0.87450227999999997</v>
+      </c>
+      <c r="Q9" s="129">
+        <v>7.3025141800000002</v>
+      </c>
+      <c r="R9" s="129">
+        <v>1.0336339400000001</v>
+      </c>
+      <c r="S9" s="141">
+        <v>7.3789210299999999</v>
+      </c>
+    </row>
+    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A10" s="91" t="s">
+        <v>351</v>
+      </c>
+      <c r="B10" s="81">
+        <v>0.69055515999999995</v>
+      </c>
+      <c r="C10" s="81">
+        <v>2.7899343399999998</v>
+      </c>
+      <c r="D10" s="81">
+        <v>0.71517302999999999</v>
+      </c>
+      <c r="E10" s="81">
+        <v>2.7196440399999999</v>
+      </c>
+      <c r="F10" s="81">
+        <v>0.68129333000000003</v>
+      </c>
+      <c r="G10" s="81">
+        <v>2.81641305</v>
+      </c>
+      <c r="H10" s="81">
+        <v>0.79046057000000003</v>
+      </c>
+      <c r="I10" s="82">
+        <v>2.8860989099999999</v>
+      </c>
+      <c r="K10" s="135">
+        <v>2013</v>
+      </c>
+      <c r="L10" s="128">
+        <v>0.79</v>
+      </c>
+      <c r="M10" s="128">
+        <v>2.34</v>
+      </c>
+      <c r="N10" s="128">
+        <v>0.87</v>
+      </c>
+      <c r="O10" s="128">
+        <v>2.6</v>
+      </c>
+      <c r="P10" s="128">
+        <v>0.74</v>
+      </c>
+      <c r="Q10" s="128">
+        <v>2.1800000000000002</v>
+      </c>
+      <c r="R10" s="128">
+        <v>0.9</v>
+      </c>
+      <c r="S10" s="142">
+        <v>2.68</v>
+      </c>
+    </row>
+    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A11" s="92" t="s">
+        <v>352</v>
+      </c>
+      <c r="B11" s="93">
+        <v>0.89105637000000004</v>
+      </c>
+      <c r="C11" s="93">
+        <v>5.0146719400000004</v>
+      </c>
+      <c r="D11" s="93">
+        <v>0.77011090999999998</v>
+      </c>
+      <c r="E11" s="93">
+        <v>4.5291129699999999</v>
+      </c>
+      <c r="F11" s="93">
+        <v>0.96521427000000004</v>
+      </c>
+      <c r="G11" s="93">
+        <v>5.31404955</v>
+      </c>
+      <c r="H11" s="93">
+        <v>0.81780103999999998</v>
+      </c>
+      <c r="I11" s="83">
+        <v>4.5193474499999997</v>
+      </c>
+      <c r="K11" s="134">
+        <v>2014</v>
+      </c>
+      <c r="L11" s="129">
+        <v>0.41049524999999998</v>
+      </c>
+      <c r="M11" s="129">
+        <v>2.26330754</v>
+      </c>
+      <c r="N11" s="129">
+        <v>0.46640717999999998</v>
+      </c>
+      <c r="O11" s="129">
+        <v>2.1655826999999999</v>
+      </c>
+      <c r="P11" s="129">
+        <v>0.37742819</v>
+      </c>
+      <c r="Q11" s="129">
+        <v>2.3213850499999999</v>
+      </c>
+      <c r="R11" s="129">
+        <v>0.53414015000000004</v>
+      </c>
+      <c r="S11" s="141">
+        <v>2.5409541999999998</v>
+      </c>
+    </row>
+    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A12" s="91" t="s">
+        <v>353</v>
+      </c>
+      <c r="B12" s="81">
+        <v>0.99737463000000004</v>
+      </c>
+      <c r="C12" s="81">
+        <v>7.1627654100000004</v>
+      </c>
+      <c r="D12" s="81">
+        <v>1.03664527</v>
+      </c>
+      <c r="E12" s="81">
+        <v>7.0990995400000001</v>
+      </c>
+      <c r="F12" s="81">
+        <v>0.96730324000000001</v>
+      </c>
+      <c r="G12" s="81">
+        <v>7.2116019800000002</v>
+      </c>
+      <c r="H12" s="81">
+        <v>1.08926491</v>
+      </c>
+      <c r="I12" s="82">
+        <v>7.10094783</v>
+      </c>
+      <c r="K12" s="136">
+        <v>2015</v>
+      </c>
+      <c r="L12" s="128">
+        <v>1.0315544800000001</v>
+      </c>
+      <c r="M12" s="128">
+        <v>2.4350353500000002</v>
+      </c>
+      <c r="N12" s="128">
+        <v>0.98447253999999995</v>
+      </c>
+      <c r="O12" s="128">
+        <v>2.4100680200000002</v>
+      </c>
+      <c r="P12" s="128">
+        <v>1.05953488</v>
+      </c>
+      <c r="Q12" s="128">
+        <v>2.4499881999999999</v>
+      </c>
+      <c r="R12" s="128">
+        <v>1.0174592600000001</v>
+      </c>
+      <c r="S12" s="142">
+        <v>2.4853554999999998</v>
+      </c>
+    </row>
+    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A13" s="92" t="s">
+        <v>354</v>
+      </c>
+      <c r="B13" s="93">
+        <v>0.75857854999999996</v>
+      </c>
+      <c r="C13" s="93">
+        <v>5.54324511</v>
+      </c>
+      <c r="D13" s="93">
+        <v>0.75484965999999998</v>
+      </c>
+      <c r="E13" s="93">
+        <v>5.5316736000000004</v>
+      </c>
+      <c r="F13" s="93">
+        <v>0.91285603000000004</v>
+      </c>
+      <c r="G13" s="93">
+        <v>6.0234691199999997</v>
+      </c>
+      <c r="H13" s="93">
+        <v>0.93390035000000005</v>
+      </c>
+      <c r="I13" s="83">
+        <v>5.84317391</v>
+      </c>
+      <c r="K13" s="137">
+        <v>2016</v>
+      </c>
+      <c r="L13" s="129">
+        <v>0.95132881000000002</v>
+      </c>
+      <c r="M13" s="129">
+        <v>5.1661812200000004</v>
+      </c>
+      <c r="N13" s="129">
+        <v>1.2141297</v>
+      </c>
+      <c r="O13" s="129">
+        <v>5.11144059</v>
+      </c>
+      <c r="P13" s="129">
+        <v>0.79657551999999998</v>
+      </c>
+      <c r="Q13" s="129">
+        <v>5.1985182300000004</v>
+      </c>
+      <c r="R13" s="129">
+        <v>1.1954396</v>
+      </c>
+      <c r="S13" s="141">
+        <v>4.9637857199999997</v>
+      </c>
+    </row>
+    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A14" s="91" t="s">
+        <v>355</v>
+      </c>
+      <c r="B14" s="81">
+        <v>1.5520078900000001</v>
+      </c>
+      <c r="C14" s="81">
+        <v>8.7213951299999994</v>
+      </c>
+      <c r="D14" s="81">
+        <v>1.48635842</v>
+      </c>
+      <c r="E14" s="81">
+        <v>8.6142080100000005</v>
+      </c>
+      <c r="F14" s="81">
+        <v>1.84987444</v>
+      </c>
+      <c r="G14" s="81">
+        <v>9.20864349</v>
+      </c>
+      <c r="H14" s="81">
+        <v>1.47271083</v>
+      </c>
+      <c r="I14" s="82">
+        <v>8.2517226000000008</v>
+      </c>
+      <c r="K14" s="135">
+        <v>2017</v>
+      </c>
+      <c r="L14" s="128">
+        <v>1.27561737</v>
+      </c>
+      <c r="M14" s="128">
+        <v>3.4902872600000001</v>
+      </c>
+      <c r="N14" s="128">
+        <v>1.3031048000000001</v>
+      </c>
+      <c r="O14" s="128">
+        <v>3.7174204300000002</v>
+      </c>
+      <c r="P14" s="128">
+        <v>1.2594790300000001</v>
+      </c>
+      <c r="Q14" s="128">
+        <v>3.35610864</v>
+      </c>
+      <c r="R14" s="128">
+        <v>1.4128810599999999</v>
+      </c>
+      <c r="S14" s="142">
+        <v>3.74124817</v>
+      </c>
+    </row>
+    <row r="15" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A15" s="92" t="s">
+        <v>356</v>
+      </c>
+      <c r="B15" s="93">
+        <v>0.68492249999999999</v>
+      </c>
+      <c r="C15" s="93">
+        <v>4.5683674999999999</v>
+      </c>
+      <c r="D15" s="93">
+        <v>0.54009289000000005</v>
+      </c>
+      <c r="E15" s="93">
+        <v>4.4132597000000002</v>
+      </c>
+      <c r="F15" s="93">
+        <v>0.79286232999999995</v>
+      </c>
+      <c r="G15" s="93">
+        <v>4.6839762699999996</v>
+      </c>
+      <c r="H15" s="93">
+        <v>0.53993643000000002</v>
+      </c>
+      <c r="I15" s="83">
+        <v>4.2556961700000002</v>
+      </c>
+      <c r="K15" s="134">
+        <v>2018</v>
+      </c>
+      <c r="L15" s="129">
+        <v>0.98107078000000003</v>
+      </c>
+      <c r="M15" s="129">
+        <v>4.4676130000000001</v>
+      </c>
+      <c r="N15" s="129">
+        <v>0.96010362000000005</v>
+      </c>
+      <c r="O15" s="129">
+        <v>4.2618057699999996</v>
+      </c>
+      <c r="P15" s="129">
+        <v>0.99356297999999998</v>
+      </c>
+      <c r="Q15" s="129">
+        <v>4.5899895400000004</v>
+      </c>
+      <c r="R15" s="129">
+        <v>1.0948183300000001</v>
+      </c>
+      <c r="S15" s="141">
+        <v>4.4766174699999999</v>
+      </c>
+    </row>
+    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A16" s="91" t="s">
+        <v>357</v>
+      </c>
+      <c r="B16" s="81">
+        <v>0.58959726000000001</v>
+      </c>
+      <c r="C16" s="81">
+        <v>5.5679997500000002</v>
+      </c>
+      <c r="D16" s="81">
+        <v>0.58041366999999999</v>
+      </c>
+      <c r="E16" s="81">
+        <v>5.3498436600000003</v>
+      </c>
+      <c r="F16" s="81">
+        <v>0.61213603999999999</v>
+      </c>
+      <c r="G16" s="81">
+        <v>6.10708742</v>
+      </c>
+      <c r="H16" s="81">
+        <v>0.60508848999999998</v>
+      </c>
+      <c r="I16" s="82">
+        <v>5.41525941</v>
+      </c>
+      <c r="K16" s="135">
+        <v>2019</v>
+      </c>
+      <c r="L16" s="128">
+        <v>0.73575869999999999</v>
+      </c>
+      <c r="M16" s="128">
+        <v>2.2451193599999999</v>
+      </c>
+      <c r="N16" s="128">
+        <v>0.74835258000000004</v>
+      </c>
+      <c r="O16" s="128">
+        <v>2.29267318</v>
+      </c>
+      <c r="P16" s="128">
+        <v>0.72835848999999997</v>
+      </c>
+      <c r="Q16" s="128">
+        <v>2.21708024</v>
+      </c>
+      <c r="R16" s="128">
+        <v>0.86293319999999996</v>
+      </c>
+      <c r="S16" s="142">
+        <v>2.3556804900000001</v>
+      </c>
+    </row>
+    <row r="17" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A17" s="92" t="s">
+        <v>358</v>
+      </c>
+      <c r="B17" s="93">
+        <v>0.70728243999999996</v>
+      </c>
+      <c r="C17" s="93">
+        <v>3.6496275699999998</v>
+      </c>
+      <c r="D17" s="93">
+        <v>0.68313246999999999</v>
+      </c>
+      <c r="E17" s="93">
+        <v>3.5541007699999998</v>
+      </c>
+      <c r="F17" s="93">
+        <v>0.83170361999999998</v>
+      </c>
+      <c r="G17" s="93">
+        <v>4.1438571299999998</v>
+      </c>
+      <c r="H17" s="93">
+        <v>0.68108880000000005</v>
+      </c>
+      <c r="I17" s="83">
+        <v>3.46811062</v>
+      </c>
+      <c r="K17" s="138">
+        <v>2020</v>
+      </c>
+      <c r="L17" s="129">
+        <v>0.86624409999999996</v>
+      </c>
+      <c r="M17" s="129">
+        <v>2.9765099699999999</v>
+      </c>
+      <c r="N17" s="129">
+        <v>0.93597386000000005</v>
+      </c>
+      <c r="O17" s="129">
+        <v>3.1044360700000002</v>
+      </c>
+      <c r="P17" s="129">
+        <v>0.82500582</v>
+      </c>
+      <c r="Q17" s="129">
+        <v>2.9009204899999999</v>
+      </c>
+      <c r="R17" s="129">
+        <v>1.0105492300000001</v>
+      </c>
+      <c r="S17" s="141">
+        <v>3.3047805800000001</v>
+      </c>
+    </row>
+    <row r="18" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A18" s="91" t="s">
+        <v>359</v>
+      </c>
+      <c r="B18" s="81">
+        <v>0.83691377</v>
+      </c>
+      <c r="C18" s="81">
+        <v>6.0996370400000002</v>
+      </c>
+      <c r="D18" s="81">
+        <v>0.82710516999999995</v>
+      </c>
+      <c r="E18" s="81">
+        <v>6.1110425499999996</v>
+      </c>
+      <c r="F18" s="81">
+        <v>0.84795973000000002</v>
+      </c>
+      <c r="G18" s="81">
+        <v>6.0867985300000003</v>
+      </c>
+      <c r="H18" s="81">
+        <v>0.79693360000000002</v>
+      </c>
+      <c r="I18" s="82">
+        <v>5.8919369499999998</v>
+      </c>
+      <c r="K18" s="139">
+        <v>2021</v>
+      </c>
+      <c r="L18" s="131">
+        <v>0.78150575</v>
+      </c>
+      <c r="M18" s="131">
+        <v>4.2904800099999996</v>
+      </c>
+      <c r="N18" s="131">
+        <v>0.80362663999999995</v>
+      </c>
+      <c r="O18" s="131">
+        <v>4.4415545400000003</v>
+      </c>
+      <c r="P18" s="131">
+        <v>0.76837789000000001</v>
+      </c>
+      <c r="Q18" s="131">
+        <v>4.2008612699999999</v>
+      </c>
+      <c r="R18" s="131">
+        <v>0.86256116999999999</v>
+      </c>
+      <c r="S18" s="143">
+        <v>4.1818283300000001</v>
+      </c>
+    </row>
+    <row r="19" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A19" s="92" t="s">
+        <v>360</v>
+      </c>
+      <c r="B19" s="93">
+        <v>1.3818176499999999</v>
+      </c>
+      <c r="C19" s="93">
+        <v>6.0626039</v>
+      </c>
+      <c r="D19" s="93">
+        <v>1.3715336199999999</v>
+      </c>
+      <c r="E19" s="93">
+        <v>6.0260605700000003</v>
+      </c>
+      <c r="F19" s="93">
+        <v>1.3943856800000001</v>
+      </c>
+      <c r="G19" s="93">
+        <v>6.1072873599999999</v>
+      </c>
+      <c r="H19" s="93">
+        <v>1.4148176800000001</v>
+      </c>
+      <c r="I19" s="83">
+        <v>5.9990733299999999</v>
+      </c>
+    </row>
+    <row r="20" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A20" s="91" t="s">
+        <v>361</v>
+      </c>
+      <c r="B20" s="81">
+        <v>1.39131699</v>
+      </c>
+      <c r="C20" s="81">
+        <v>6.2504713299999999</v>
+      </c>
+      <c r="D20" s="81">
+        <v>1.40071769</v>
+      </c>
+      <c r="E20" s="81">
+        <v>5.9608757600000004</v>
+      </c>
+      <c r="F20" s="81">
+        <v>1.3876790000000001</v>
+      </c>
+      <c r="G20" s="81">
+        <v>6.3629820400000003</v>
+      </c>
+      <c r="H20" s="81">
+        <v>1.4381440299999999</v>
+      </c>
+      <c r="I20" s="82">
+        <v>5.9193692699999998</v>
+      </c>
+    </row>
+    <row r="21" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A21" s="92" t="s">
+        <v>362</v>
+      </c>
+      <c r="B21" s="93">
+        <v>0.21500121</v>
+      </c>
+      <c r="C21" s="93">
+        <v>3.6483459800000002</v>
+      </c>
+      <c r="D21" s="93">
+        <v>0.20195390999999999</v>
+      </c>
+      <c r="E21" s="93">
+        <v>3.55554557</v>
+      </c>
+      <c r="F21" s="93">
+        <v>0.24199641</v>
+      </c>
+      <c r="G21" s="93">
+        <v>3.8408045899999999</v>
+      </c>
+      <c r="H21" s="93">
+        <v>0.20594814</v>
+      </c>
+      <c r="I21" s="83">
+        <v>3.5535044099999999</v>
+      </c>
+    </row>
+    <row r="22" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A22" s="95" t="s">
+        <v>363</v>
+      </c>
+      <c r="B22" s="96">
+        <v>0.92124664000000001</v>
+      </c>
+      <c r="C22" s="96">
+        <v>4.7567849600000001</v>
+      </c>
+      <c r="D22" s="96">
+        <v>0.95045422999999996</v>
+      </c>
+      <c r="E22" s="96">
+        <v>4.42801226</v>
+      </c>
+      <c r="F22" s="96">
+        <v>0.89833116999999996</v>
+      </c>
+      <c r="G22" s="96">
+        <v>5.0163182199999996</v>
+      </c>
+      <c r="H22" s="96">
+        <v>0.99737423999999997</v>
+      </c>
+      <c r="I22" s="97">
+        <v>4.5531845899999999</v>
+      </c>
+    </row>
+    <row r="24" spans="1:19" ht="20.25" x14ac:dyDescent="0.25">
+      <c r="A24" s="73" t="s">
+        <v>339</v>
+      </c>
+      <c r="B24" s="72"/>
+      <c r="C24" s="72"/>
+      <c r="D24" s="72"/>
+      <c r="E24" s="72"/>
+      <c r="F24" s="72"/>
+      <c r="G24" s="72"/>
+      <c r="H24" s="72"/>
+      <c r="I24" s="72"/>
+      <c r="J24" s="72"/>
+      <c r="K24" s="72"/>
+      <c r="L24" s="72"/>
+      <c r="M24" s="72"/>
+      <c r="N24" s="72"/>
+      <c r="O24" s="72"/>
+      <c r="P24" s="72"/>
+    </row>
+    <row r="25" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A25" s="106" t="s">
+        <v>364</v>
+      </c>
+      <c r="B25" s="105"/>
+      <c r="C25" s="105"/>
+      <c r="D25" s="105"/>
+      <c r="E25" s="105"/>
+      <c r="F25" s="105"/>
+      <c r="G25" s="105"/>
+      <c r="H25" s="105"/>
+      <c r="I25" s="105"/>
+      <c r="J25" s="105"/>
+      <c r="K25" s="105"/>
+      <c r="L25" s="105"/>
+      <c r="M25" s="105"/>
+      <c r="N25" s="105"/>
+      <c r="O25" s="105"/>
+      <c r="P25" s="105"/>
+    </row>
+    <row r="26" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A26" s="113"/>
+      <c r="B26" s="113"/>
+      <c r="C26" s="113"/>
+      <c r="D26" s="113"/>
+      <c r="E26" s="113"/>
+      <c r="F26" s="113"/>
+      <c r="G26" s="113"/>
+      <c r="H26" s="113"/>
+      <c r="I26" s="113"/>
+      <c r="J26" s="113"/>
+      <c r="K26" s="113"/>
+      <c r="L26" s="113"/>
+      <c r="M26" s="113"/>
+      <c r="N26" s="113"/>
+      <c r="O26" s="113"/>
+      <c r="P26" s="113"/>
+    </row>
+    <row r="27" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A27" s="114" t="s">
+        <v>365</v>
+      </c>
+      <c r="B27" s="104" t="s">
+        <v>346</v>
+      </c>
+      <c r="C27" s="75"/>
+      <c r="D27" s="75"/>
+      <c r="E27" s="75"/>
+      <c r="F27" s="75"/>
+      <c r="G27" s="104" t="s">
+        <v>366</v>
+      </c>
+      <c r="H27" s="75"/>
+      <c r="I27" s="75"/>
+      <c r="J27" s="75"/>
+      <c r="K27" s="103"/>
+      <c r="L27" s="102" t="s">
+        <v>347</v>
+      </c>
+      <c r="M27" s="101"/>
+      <c r="N27" s="101"/>
+      <c r="O27" s="101"/>
+      <c r="P27" s="100"/>
+    </row>
+    <row r="28" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A28" s="108"/>
+      <c r="B28" s="115">
+        <v>2017</v>
+      </c>
+      <c r="C28" s="115">
+        <v>2018</v>
+      </c>
+      <c r="D28" s="115">
+        <v>2019</v>
+      </c>
+      <c r="E28" s="120">
+        <v>2020</v>
+      </c>
+      <c r="F28" s="120">
+        <v>2021</v>
+      </c>
+      <c r="G28" s="108">
+        <v>2017</v>
+      </c>
+      <c r="H28" s="115">
+        <v>2018</v>
+      </c>
+      <c r="I28" s="115">
+        <v>2019</v>
+      </c>
+      <c r="J28" s="115">
+        <v>2020</v>
+      </c>
+      <c r="K28" s="120">
+        <v>2021</v>
+      </c>
+      <c r="L28" s="108">
+        <v>2017</v>
+      </c>
+      <c r="M28" s="115">
+        <v>2018</v>
+      </c>
+      <c r="N28" s="115">
+        <v>2019</v>
+      </c>
+      <c r="O28" s="115">
+        <v>2020</v>
+      </c>
+      <c r="P28" s="120">
+        <v>2021</v>
+      </c>
+    </row>
+    <row r="29" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A29" s="116" t="s">
+        <v>367</v>
+      </c>
+      <c r="B29" s="116">
+        <v>1.27561737</v>
+      </c>
+      <c r="C29" s="111">
+        <v>0.98107078000000003</v>
+      </c>
+      <c r="D29" s="111">
+        <v>0.73575869999999999</v>
+      </c>
+      <c r="E29" s="111">
+        <v>0.86624409999999996</v>
+      </c>
+      <c r="F29" s="109">
+        <v>0.78150575</v>
+      </c>
+      <c r="G29" s="111">
+        <v>1.27561737</v>
+      </c>
+      <c r="H29" s="117">
+        <v>0.98107078000000003</v>
+      </c>
+      <c r="I29" s="117">
+        <v>0.73575869999999999</v>
+      </c>
+      <c r="J29" s="117">
+        <v>0.86624409999999996</v>
+      </c>
+      <c r="K29" s="110">
+        <v>0.78150575</v>
+      </c>
+      <c r="L29" s="117">
+        <v>3.4902872600000001</v>
+      </c>
+      <c r="M29" s="117">
+        <v>4.4676130000000001</v>
+      </c>
+      <c r="N29" s="117">
+        <v>2.2451193599999999</v>
+      </c>
+      <c r="O29" s="117">
+        <v>2.9765099699999999</v>
+      </c>
+      <c r="P29" s="110">
+        <v>4.2904800099999996</v>
+      </c>
+    </row>
+    <row r="30" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A30" s="118" t="s">
+        <v>368</v>
+      </c>
+      <c r="B30" s="118">
+        <v>1.7046296400000001</v>
+      </c>
+      <c r="C30" s="107">
+        <v>0.47</v>
+      </c>
+      <c r="D30" s="107">
+        <v>0.59904170999999995</v>
+      </c>
+      <c r="E30" s="107">
+        <v>0.89852845999999997</v>
+      </c>
+      <c r="F30" s="107"/>
+      <c r="G30" s="107">
+        <v>3.0019915699999999</v>
+      </c>
+      <c r="H30" s="107">
+        <v>1.46</v>
+      </c>
+      <c r="I30" s="107">
+        <v>1.3392079100000001</v>
+      </c>
+      <c r="J30" s="107">
+        <v>1.77255601</v>
+      </c>
+      <c r="K30" s="107"/>
+      <c r="L30" s="107">
+        <v>4.1945793900000004</v>
+      </c>
+      <c r="M30" s="107">
+        <v>3.2</v>
+      </c>
+      <c r="N30" s="107">
+        <v>2.3749285499999999</v>
+      </c>
+      <c r="O30" s="107">
+        <v>3.28307452</v>
+      </c>
+      <c r="P30" s="107"/>
+    </row>
+    <row r="31" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A31" s="116" t="s">
+        <v>369</v>
+      </c>
+      <c r="B31" s="116">
+        <v>0.63853875000000004</v>
+      </c>
+      <c r="C31" s="111">
+        <v>0.36856003999999998</v>
+      </c>
+      <c r="D31" s="111">
+        <v>0.46673712000000001</v>
+      </c>
+      <c r="E31" s="111">
+        <v>0.37425488000000001</v>
+      </c>
+      <c r="F31" s="111"/>
+      <c r="G31" s="111">
+        <v>3.65969919</v>
+      </c>
+      <c r="H31" s="111">
+        <v>1.83111132</v>
+      </c>
+      <c r="I31" s="111">
+        <v>1.81219562</v>
+      </c>
+      <c r="J31" s="111">
+        <v>2.1534447700000001</v>
+      </c>
+      <c r="K31" s="111"/>
+      <c r="L31" s="111">
+        <v>4.2961077100000002</v>
+      </c>
+      <c r="M31" s="111">
+        <v>2.9241143100000002</v>
+      </c>
+      <c r="N31" s="111">
+        <v>2.47506819</v>
+      </c>
+      <c r="O31" s="111">
+        <v>3.1879997699999998</v>
+      </c>
+      <c r="P31" s="111"/>
+    </row>
+    <row r="32" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A32" s="118" t="s">
+        <v>370</v>
+      </c>
+      <c r="B32" s="118">
+        <v>6.7543210000000006E-2</v>
+      </c>
+      <c r="C32" s="107">
+        <v>0.13822229</v>
+      </c>
+      <c r="D32" s="107">
+        <v>9.8963809999999999E-2</v>
+      </c>
+      <c r="E32" s="107">
+        <v>0.32812571000000001</v>
+      </c>
+      <c r="F32" s="107"/>
+      <c r="G32" s="107">
+        <v>3.72971428</v>
+      </c>
+      <c r="H32" s="107">
+        <v>1.9718646099999999</v>
+      </c>
+      <c r="I32" s="107">
+        <v>1.9129528499999999</v>
+      </c>
+      <c r="J32" s="107">
+        <v>2.4886364900000002</v>
+      </c>
+      <c r="K32" s="107"/>
+      <c r="L32" s="107">
+        <v>4.0357390300000002</v>
+      </c>
+      <c r="M32" s="107">
+        <v>2.99681102</v>
+      </c>
+      <c r="N32" s="107">
+        <v>2.4348935599999999</v>
+      </c>
+      <c r="O32" s="107">
+        <v>3.4242335700000002</v>
+      </c>
+      <c r="P32" s="107"/>
+    </row>
+    <row r="33" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A33" s="116" t="s">
+        <v>371</v>
+      </c>
+      <c r="B33" s="116">
+        <v>4.192655E-2</v>
+      </c>
+      <c r="C33" s="111">
+        <v>0.15155073999999999</v>
+      </c>
+      <c r="D33" s="111">
+        <v>8.7270619999999993E-2</v>
+      </c>
+      <c r="E33" s="111">
+        <v>9.2740320000000001E-2</v>
+      </c>
+      <c r="F33" s="111"/>
+      <c r="G33" s="111">
+        <v>3.7732045699999999</v>
+      </c>
+      <c r="H33" s="111">
+        <v>2.1264037199999999</v>
+      </c>
+      <c r="I33" s="111">
+        <v>2.00189291</v>
+      </c>
+      <c r="J33" s="111">
+        <v>2.58368478</v>
+      </c>
+      <c r="K33" s="111"/>
+      <c r="L33" s="111">
+        <v>3.7191104199999998</v>
+      </c>
+      <c r="M33" s="111">
+        <v>3.1096731200000001</v>
+      </c>
+      <c r="N33" s="111">
+        <v>2.36914793</v>
+      </c>
+      <c r="O33" s="111">
+        <v>3.4298856400000002</v>
+      </c>
+      <c r="P33" s="111"/>
+    </row>
+    <row r="34" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A34" s="118" t="s">
+        <v>372</v>
+      </c>
+      <c r="B34" s="118">
+        <v>-9.8829490000000006E-2</v>
+      </c>
+      <c r="C34" s="107">
+        <v>0.10167846</v>
+      </c>
+      <c r="D34" s="107">
+        <v>8.4050650000000005E-2</v>
+      </c>
+      <c r="E34" s="107">
+        <v>0.19827358</v>
+      </c>
+      <c r="F34" s="107"/>
+      <c r="G34" s="107">
+        <v>3.6706460399999998</v>
+      </c>
+      <c r="H34" s="107">
+        <v>2.23024427</v>
+      </c>
+      <c r="I34" s="107">
+        <v>2.0876261600000001</v>
+      </c>
+      <c r="J34" s="107">
+        <v>2.7870811299999998</v>
+      </c>
+      <c r="K34" s="107"/>
+      <c r="L34" s="107">
+        <v>3.5409220399999999</v>
+      </c>
+      <c r="M34" s="107">
+        <v>3.3166207399999998</v>
+      </c>
+      <c r="N34" s="107">
+        <v>2.3511208199999998</v>
+      </c>
+      <c r="O34" s="107">
+        <v>3.5479270600000001</v>
+      </c>
+      <c r="P34" s="107"/>
+    </row>
+    <row r="35" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A35" s="116" t="s">
+        <v>373</v>
+      </c>
+      <c r="B35" s="116">
+        <v>1.6411019999999998E-2</v>
+      </c>
+      <c r="C35" s="111">
+        <v>1.8854030000000001E-2</v>
+      </c>
+      <c r="D35" s="111">
+        <v>0.18865905999999999</v>
+      </c>
+      <c r="E35" s="111">
+        <v>9.4755989999999998E-2</v>
+      </c>
+      <c r="F35" s="111"/>
+      <c r="G35" s="111">
+        <v>3.6876594499999999</v>
+      </c>
+      <c r="H35" s="111">
+        <v>2.2495187900000002</v>
+      </c>
+      <c r="I35" s="111">
+        <v>2.28022372</v>
+      </c>
+      <c r="J35" s="111">
+        <v>2.8844780399999999</v>
+      </c>
+      <c r="K35" s="111"/>
+      <c r="L35" s="111">
+        <v>3.5209647300000002</v>
+      </c>
+      <c r="M35" s="111">
+        <v>3.3191443600000001</v>
+      </c>
+      <c r="N35" s="111">
+        <v>2.5248854199999999</v>
+      </c>
+      <c r="O35" s="111">
+        <v>3.4508754800000001</v>
+      </c>
+      <c r="P35" s="111"/>
+    </row>
+    <row r="36" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A36" s="118" t="s">
+        <v>374</v>
+      </c>
+      <c r="B36" s="118">
+        <v>2.3834629999999999E-2</v>
+      </c>
+      <c r="C36" s="107">
+        <v>5.7494999999999996E-4</v>
+      </c>
+      <c r="D36" s="107">
+        <v>8.9809269999999997E-2</v>
+      </c>
+      <c r="E36" s="107">
+        <v>0.1358789</v>
+      </c>
+      <c r="F36" s="107"/>
+      <c r="G36" s="107">
+        <v>3.7123730199999998</v>
+      </c>
+      <c r="H36" s="107">
+        <v>2.2501066700000001</v>
+      </c>
+      <c r="I36" s="107">
+        <v>2.3720808400000002</v>
+      </c>
+      <c r="J36" s="107">
+        <v>3.0242763400000001</v>
+      </c>
+      <c r="K36" s="107"/>
+      <c r="L36" s="107">
+        <v>3.4573656399999999</v>
+      </c>
+      <c r="M36" s="107">
+        <v>3.2951183799999999</v>
+      </c>
+      <c r="N36" s="107">
+        <v>2.6163722699999998</v>
+      </c>
+      <c r="O36" s="107">
+        <v>3.4984921600000001</v>
+      </c>
+      <c r="P36" s="107"/>
+    </row>
+    <row r="37" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A37" s="116" t="s">
+        <v>375</v>
+      </c>
+      <c r="B37" s="116">
+        <v>0.26636274999999998</v>
+      </c>
+      <c r="C37" s="111">
+        <v>8.7425089999999997E-2</v>
+      </c>
+      <c r="D37" s="111">
+        <v>0.17346186999999999</v>
+      </c>
+      <c r="E37" s="111">
+        <v>0.2111392</v>
+      </c>
+      <c r="F37" s="111"/>
+      <c r="G37" s="111">
+        <v>3.9886241500000001</v>
+      </c>
+      <c r="H37" s="111">
+        <v>2.33949892</v>
+      </c>
+      <c r="I37" s="111">
+        <v>2.5496573599999999</v>
+      </c>
+      <c r="J37" s="111">
+        <v>3.2418009699999999</v>
+      </c>
+      <c r="K37" s="111"/>
+      <c r="L37" s="111">
+        <v>3.6873149000000001</v>
+      </c>
+      <c r="M37" s="111">
+        <v>3.1107755300000002</v>
+      </c>
+      <c r="N37" s="111">
+        <v>2.7045829800000001</v>
+      </c>
+      <c r="O37" s="111">
+        <v>3.5374200899999999</v>
+      </c>
+      <c r="P37" s="111"/>
+    </row>
+    <row r="38" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A38" s="118" t="s">
+        <v>376</v>
+      </c>
+      <c r="B38" s="118">
+        <v>0.32512827</v>
+      </c>
+      <c r="C38" s="107">
+        <v>-2.5840209999999999E-2</v>
+      </c>
+      <c r="D38" s="107">
+        <v>0.15021355</v>
+      </c>
+      <c r="E38" s="107">
+        <v>0.26810007000000002</v>
+      </c>
+      <c r="F38" s="107"/>
+      <c r="G38" s="107">
+        <v>4.32672056</v>
+      </c>
+      <c r="H38" s="107">
+        <v>2.3130541899999999</v>
+      </c>
+      <c r="I38" s="107">
+        <v>2.7037008400000002</v>
+      </c>
+      <c r="J38" s="107">
+        <v>3.5185923099999998</v>
+      </c>
+      <c r="K38" s="107"/>
+      <c r="L38" s="107">
+        <v>4.1314744399999999</v>
+      </c>
+      <c r="M38" s="107">
+        <v>2.7500619999999998</v>
+      </c>
+      <c r="N38" s="107">
+        <v>2.8854449799999999</v>
+      </c>
+      <c r="O38" s="107">
+        <v>3.6592936900000002</v>
+      </c>
+      <c r="P38" s="107"/>
+    </row>
+    <row r="39" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A39" s="116" t="s">
+        <v>377</v>
+      </c>
+      <c r="B39" s="116">
+        <v>0.24821524</v>
+      </c>
+      <c r="C39" s="111">
+        <v>8.7129579999999998E-2</v>
+      </c>
+      <c r="D39" s="111">
+        <v>3.2538419999999998E-2</v>
+      </c>
+      <c r="E39" s="111">
+        <v>0.34408348</v>
+      </c>
+      <c r="F39" s="111"/>
+      <c r="G39" s="111">
+        <v>4.5856753799999996</v>
+      </c>
+      <c r="H39" s="111">
+        <v>2.4021991200000001</v>
+      </c>
+      <c r="I39" s="111">
+        <v>2.7371189999999999</v>
+      </c>
+      <c r="J39" s="111">
+        <v>3.87478268</v>
+      </c>
+      <c r="K39" s="111"/>
+      <c r="L39" s="111">
+        <v>4.5457282799999996</v>
+      </c>
+      <c r="M39" s="111">
+        <v>2.5849562000000001</v>
+      </c>
+      <c r="N39" s="111">
+        <v>2.8293275200000001</v>
+      </c>
+      <c r="O39" s="111">
+        <v>3.98213405</v>
+      </c>
+      <c r="P39" s="111"/>
+    </row>
+    <row r="40" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A40" s="119" t="s">
+        <v>378</v>
+      </c>
+      <c r="B40" s="119">
+        <v>0.17846988</v>
+      </c>
+      <c r="C40" s="112">
+        <v>8.9751910000000004E-2</v>
+      </c>
+      <c r="D40" s="112">
+        <v>0.10334690000000001</v>
+      </c>
+      <c r="E40" s="112">
+        <v>0.48460853999999998</v>
+      </c>
+      <c r="F40" s="121"/>
+      <c r="G40" s="112">
+        <v>4.7723293099999999</v>
+      </c>
+      <c r="H40" s="112">
+        <v>2.4941070399999998</v>
+      </c>
+      <c r="I40" s="112">
+        <v>2.8432946299999999</v>
+      </c>
+      <c r="J40" s="112">
+        <v>4.3781687500000004</v>
+      </c>
+      <c r="K40" s="121"/>
+      <c r="L40" s="112">
+        <v>4.7723293099999999</v>
+      </c>
+      <c r="M40" s="112">
+        <v>2.4941070399999998</v>
+      </c>
+      <c r="N40" s="112">
+        <v>2.8432946299999999</v>
+      </c>
+      <c r="O40" s="112">
+        <v>4.3781687500000004</v>
+      </c>
+      <c r="P40" s="121"/>
+    </row>
+  </sheetData>
+  <mergeCells count="19">
+    <mergeCell ref="A1:I1"/>
+    <mergeCell ref="A2:I2"/>
+    <mergeCell ref="A24:P24"/>
+    <mergeCell ref="A25:P25"/>
+    <mergeCell ref="B27:F27"/>
+    <mergeCell ref="G27:K27"/>
+    <mergeCell ref="L27:P27"/>
+    <mergeCell ref="K3:S3"/>
+    <mergeCell ref="P5:Q5"/>
+    <mergeCell ref="R5:S5"/>
+    <mergeCell ref="K1:S1"/>
+    <mergeCell ref="K2:S2"/>
+    <mergeCell ref="N5:O5"/>
+    <mergeCell ref="L5:M5"/>
+    <mergeCell ref="H5:I5"/>
+    <mergeCell ref="A3:I3"/>
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="D5:E5"/>
+    <mergeCell ref="F5:G5"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{66AF708D-74D2-4120-834F-8C98B2607E50}">
   <dimension ref="A1:M1193"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K1" sqref="K1"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -56554,11 +59372,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B823923B-B32A-4DEA-A2A8-D5975B65A271}">
   <dimension ref="A1:H952"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="N13" sqref="N13"/>
     </sheetView>
   </sheetViews>
@@ -82271,688 +85089,4 @@
   <autoFilter ref="A1:H952" xr:uid="{B823923B-B32A-4DEA-A2A8-D5975B65A271}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9F45B1B4-192A-4769-AF8C-9EA5A2391269}">
-  <dimension ref="A1:I49"/>
-  <sheetViews>
-    <sheetView topLeftCell="A32" workbookViewId="0">
-      <selection activeCell="C39" sqref="C39:C44"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" s="34"/>
-      <c r="B1" s="34"/>
-      <c r="C1" s="34"/>
-      <c r="D1" s="34"/>
-      <c r="E1" s="34"/>
-      <c r="F1" s="34"/>
-      <c r="G1" s="34"/>
-      <c r="H1" s="34"/>
-      <c r="I1" s="34"/>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" s="34"/>
-      <c r="B2" s="34"/>
-      <c r="C2" s="34"/>
-      <c r="D2" s="34"/>
-      <c r="E2" s="34"/>
-      <c r="F2" s="34"/>
-      <c r="G2" s="34"/>
-      <c r="H2" s="34"/>
-      <c r="I2" s="34"/>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" s="62" t="s">
-        <v>49</v>
-      </c>
-      <c r="B3" s="63"/>
-      <c r="C3" s="63"/>
-      <c r="D3" s="63"/>
-      <c r="E3" s="63"/>
-      <c r="F3" s="63"/>
-      <c r="G3" s="63"/>
-      <c r="H3" s="63"/>
-      <c r="I3" s="63"/>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" s="64"/>
-      <c r="B4" s="65"/>
-      <c r="C4" s="65"/>
-      <c r="D4" s="65"/>
-      <c r="E4" s="65"/>
-      <c r="F4" s="65"/>
-      <c r="G4" s="65"/>
-      <c r="H4" s="65"/>
-      <c r="I4" s="65"/>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" s="66" t="s">
-        <v>50</v>
-      </c>
-      <c r="B5" s="66"/>
-      <c r="C5" s="66"/>
-      <c r="D5" s="66"/>
-      <c r="E5" s="66"/>
-      <c r="F5" s="66"/>
-      <c r="G5" s="66"/>
-      <c r="H5" s="66"/>
-      <c r="I5" s="66"/>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" s="67"/>
-      <c r="B6" s="67"/>
-      <c r="C6" s="67"/>
-      <c r="D6" s="67"/>
-      <c r="E6" s="67"/>
-      <c r="F6" s="67"/>
-      <c r="G6" s="67"/>
-      <c r="H6" s="67"/>
-      <c r="I6" s="67"/>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7" s="67"/>
-      <c r="B7" s="67"/>
-      <c r="C7" s="67"/>
-      <c r="D7" s="67"/>
-      <c r="E7" s="67"/>
-      <c r="F7" s="67"/>
-      <c r="G7" s="67"/>
-      <c r="H7" s="67"/>
-      <c r="I7" s="67"/>
-    </row>
-    <row r="8" spans="1:9" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A8" s="35"/>
-      <c r="B8" s="36"/>
-      <c r="C8" s="35"/>
-      <c r="D8" s="35"/>
-      <c r="E8" s="35"/>
-      <c r="F8" s="35"/>
-      <c r="G8" s="35"/>
-      <c r="H8" s="35"/>
-      <c r="I8" s="35"/>
-    </row>
-    <row r="9" spans="1:9" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A9" s="35"/>
-      <c r="B9" s="37" t="s">
-        <v>28</v>
-      </c>
-      <c r="C9" s="38"/>
-      <c r="D9" s="38"/>
-      <c r="E9" s="35"/>
-      <c r="F9" s="35"/>
-      <c r="G9" s="35"/>
-      <c r="H9" s="35"/>
-      <c r="I9" s="35"/>
-    </row>
-    <row r="10" spans="1:9" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A10" s="35"/>
-      <c r="B10" s="38" t="s">
-        <v>51</v>
-      </c>
-      <c r="C10" s="38"/>
-      <c r="D10" s="38"/>
-      <c r="E10" s="35"/>
-      <c r="F10" s="35"/>
-      <c r="G10" s="35"/>
-      <c r="H10" s="35"/>
-      <c r="I10" s="35"/>
-    </row>
-    <row r="11" spans="1:9" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A11" s="35"/>
-      <c r="B11" s="38"/>
-      <c r="C11" s="38"/>
-      <c r="D11" s="38"/>
-      <c r="E11" s="35"/>
-      <c r="F11" s="35"/>
-      <c r="G11" s="35"/>
-      <c r="H11" s="35"/>
-      <c r="I11" s="35"/>
-    </row>
-    <row r="12" spans="1:9" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A12" s="35"/>
-      <c r="B12" s="37" t="s">
-        <v>29</v>
-      </c>
-      <c r="C12" s="38"/>
-      <c r="D12" s="38"/>
-      <c r="E12" s="35"/>
-      <c r="F12" s="35"/>
-      <c r="G12" s="35"/>
-      <c r="H12" s="35"/>
-      <c r="I12" s="35"/>
-    </row>
-    <row r="13" spans="1:9" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A13" s="35"/>
-      <c r="B13" s="38" t="s">
-        <v>52</v>
-      </c>
-      <c r="C13" s="38"/>
-      <c r="D13" s="38"/>
-      <c r="E13" s="35"/>
-      <c r="F13" s="35"/>
-      <c r="G13" s="35"/>
-      <c r="H13" s="35"/>
-      <c r="I13" s="35"/>
-    </row>
-    <row r="14" spans="1:9" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A14" s="35"/>
-      <c r="B14" s="38"/>
-      <c r="C14" s="38"/>
-      <c r="D14" s="38"/>
-      <c r="E14" s="35"/>
-      <c r="F14" s="35"/>
-      <c r="G14" s="35"/>
-      <c r="H14" s="35"/>
-      <c r="I14" s="35"/>
-    </row>
-    <row r="15" spans="1:9" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A15" s="35"/>
-      <c r="B15" s="37" t="s">
-        <v>53</v>
-      </c>
-      <c r="C15" s="38"/>
-      <c r="D15" s="38"/>
-      <c r="E15" s="35"/>
-      <c r="F15" s="35"/>
-      <c r="G15" s="35"/>
-      <c r="H15" s="35"/>
-      <c r="I15" s="35"/>
-    </row>
-    <row r="16" spans="1:9" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A16" s="35"/>
-      <c r="B16" s="38">
-        <v>1</v>
-      </c>
-      <c r="C16" s="38" t="s">
-        <v>54</v>
-      </c>
-      <c r="D16" s="38"/>
-      <c r="E16" s="35"/>
-      <c r="F16" s="35"/>
-      <c r="G16" s="35"/>
-      <c r="H16" s="35"/>
-      <c r="I16" s="35"/>
-    </row>
-    <row r="17" spans="1:9" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A17" s="35"/>
-      <c r="B17" s="38">
-        <v>2</v>
-      </c>
-      <c r="C17" s="38" t="s">
-        <v>55</v>
-      </c>
-      <c r="D17" s="38"/>
-      <c r="E17" s="35"/>
-      <c r="F17" s="35"/>
-      <c r="G17" s="35"/>
-      <c r="H17" s="35"/>
-      <c r="I17" s="35"/>
-    </row>
-    <row r="18" spans="1:9" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A18" s="35"/>
-      <c r="B18" s="38">
-        <v>3</v>
-      </c>
-      <c r="C18" s="38" t="s">
-        <v>56</v>
-      </c>
-      <c r="D18" s="38"/>
-      <c r="E18" s="35"/>
-      <c r="F18" s="35"/>
-      <c r="G18" s="35"/>
-      <c r="H18" s="35"/>
-      <c r="I18" s="35"/>
-    </row>
-    <row r="19" spans="1:9" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A19" s="35"/>
-      <c r="B19" s="38">
-        <v>4</v>
-      </c>
-      <c r="C19" s="38" t="s">
-        <v>57</v>
-      </c>
-      <c r="D19" s="38"/>
-      <c r="E19" s="35"/>
-      <c r="F19" s="35"/>
-      <c r="G19" s="35"/>
-      <c r="H19" s="35"/>
-      <c r="I19" s="35"/>
-    </row>
-    <row r="20" spans="1:9" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A20" s="35"/>
-      <c r="B20" s="38">
-        <v>5</v>
-      </c>
-      <c r="C20" s="38" t="s">
-        <v>58</v>
-      </c>
-      <c r="D20" s="38"/>
-      <c r="E20" s="35"/>
-      <c r="F20" s="35"/>
-      <c r="G20" s="35"/>
-      <c r="H20" s="35"/>
-      <c r="I20" s="35"/>
-    </row>
-    <row r="21" spans="1:9" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A21" s="35"/>
-      <c r="B21" s="38">
-        <v>6</v>
-      </c>
-      <c r="C21" s="38" t="s">
-        <v>59</v>
-      </c>
-      <c r="D21" s="38"/>
-      <c r="E21" s="35"/>
-      <c r="F21" s="35"/>
-      <c r="G21" s="35"/>
-      <c r="H21" s="35"/>
-      <c r="I21" s="35"/>
-    </row>
-    <row r="22" spans="1:9" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A22" s="35"/>
-      <c r="B22" s="38">
-        <v>7</v>
-      </c>
-      <c r="C22" s="38" t="s">
-        <v>60</v>
-      </c>
-      <c r="D22" s="38"/>
-      <c r="E22" s="35"/>
-      <c r="F22" s="35"/>
-      <c r="G22" s="35"/>
-      <c r="H22" s="35"/>
-      <c r="I22" s="35"/>
-    </row>
-    <row r="23" spans="1:9" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A23" s="35"/>
-      <c r="B23" s="38">
-        <v>8</v>
-      </c>
-      <c r="C23" s="38" t="s">
-        <v>61</v>
-      </c>
-      <c r="D23" s="38"/>
-      <c r="E23" s="35"/>
-      <c r="F23" s="35"/>
-      <c r="G23" s="35"/>
-      <c r="H23" s="35"/>
-      <c r="I23" s="35"/>
-    </row>
-    <row r="24" spans="1:9" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A24" s="35"/>
-      <c r="B24" s="38">
-        <v>9</v>
-      </c>
-      <c r="C24" s="38" t="s">
-        <v>62</v>
-      </c>
-      <c r="D24" s="38"/>
-      <c r="E24" s="35"/>
-      <c r="F24" s="35"/>
-      <c r="G24" s="35"/>
-      <c r="H24" s="35"/>
-      <c r="I24" s="35"/>
-    </row>
-    <row r="25" spans="1:9" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A25" s="35"/>
-      <c r="B25" s="38">
-        <v>10</v>
-      </c>
-      <c r="C25" s="38" t="s">
-        <v>63</v>
-      </c>
-      <c r="D25" s="38"/>
-      <c r="E25" s="35"/>
-      <c r="F25" s="35"/>
-      <c r="G25" s="35"/>
-      <c r="H25" s="35"/>
-      <c r="I25" s="35"/>
-    </row>
-    <row r="26" spans="1:9" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A26" s="35"/>
-      <c r="B26" s="38">
-        <v>11</v>
-      </c>
-      <c r="C26" s="38" t="s">
-        <v>64</v>
-      </c>
-      <c r="D26" s="38"/>
-      <c r="E26" s="35"/>
-      <c r="F26" s="35"/>
-      <c r="G26" s="35"/>
-      <c r="H26" s="35"/>
-      <c r="I26" s="35"/>
-    </row>
-    <row r="27" spans="1:9" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A27" s="35"/>
-      <c r="B27" s="38">
-        <v>12</v>
-      </c>
-      <c r="C27" s="38" t="s">
-        <v>65</v>
-      </c>
-      <c r="D27" s="38"/>
-      <c r="E27" s="35"/>
-      <c r="F27" s="35"/>
-      <c r="G27" s="35"/>
-      <c r="H27" s="35"/>
-      <c r="I27" s="35"/>
-    </row>
-    <row r="28" spans="1:9" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A28" s="35"/>
-      <c r="B28" s="38"/>
-      <c r="C28" s="38"/>
-      <c r="D28" s="38"/>
-      <c r="E28" s="35"/>
-      <c r="F28" s="35"/>
-      <c r="G28" s="35"/>
-      <c r="H28" s="35"/>
-      <c r="I28" s="35"/>
-    </row>
-    <row r="29" spans="1:9" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A29" s="35"/>
-      <c r="B29" s="37" t="s">
-        <v>30</v>
-      </c>
-      <c r="C29" s="38"/>
-      <c r="D29" s="38"/>
-      <c r="E29" s="35"/>
-      <c r="F29" s="35"/>
-      <c r="G29" s="35"/>
-      <c r="H29" s="35"/>
-      <c r="I29" s="35"/>
-    </row>
-    <row r="30" spans="1:9" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A30" s="35"/>
-      <c r="B30" s="38">
-        <v>1</v>
-      </c>
-      <c r="C30" s="38" t="s">
-        <v>66</v>
-      </c>
-      <c r="D30" s="38"/>
-      <c r="E30" s="35"/>
-      <c r="F30" s="35"/>
-      <c r="G30" s="35"/>
-      <c r="H30" s="35"/>
-      <c r="I30" s="35"/>
-    </row>
-    <row r="31" spans="1:9" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A31" s="35"/>
-      <c r="B31" s="38">
-        <v>2</v>
-      </c>
-      <c r="C31" s="38" t="s">
-        <v>67</v>
-      </c>
-      <c r="D31" s="38"/>
-      <c r="E31" s="35"/>
-      <c r="F31" s="35"/>
-      <c r="G31" s="35"/>
-      <c r="H31" s="35"/>
-      <c r="I31" s="35"/>
-    </row>
-    <row r="32" spans="1:9" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A32" s="35"/>
-      <c r="B32" s="38"/>
-      <c r="C32" s="38"/>
-      <c r="D32" s="38"/>
-      <c r="E32" s="35"/>
-      <c r="F32" s="35"/>
-      <c r="G32" s="35"/>
-      <c r="H32" s="35"/>
-      <c r="I32" s="35"/>
-    </row>
-    <row r="33" spans="1:9" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A33" s="35"/>
-      <c r="B33" s="37" t="s">
-        <v>31</v>
-      </c>
-      <c r="C33" s="38"/>
-      <c r="D33" s="38"/>
-      <c r="E33" s="35"/>
-      <c r="F33" s="35"/>
-      <c r="G33" s="35"/>
-      <c r="H33" s="35"/>
-      <c r="I33" s="35"/>
-    </row>
-    <row r="34" spans="1:9" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A34" s="35"/>
-      <c r="B34" s="38">
-        <v>1</v>
-      </c>
-      <c r="C34" s="38" t="s">
-        <v>68</v>
-      </c>
-      <c r="D34" s="38"/>
-      <c r="E34" s="35"/>
-      <c r="F34" s="35"/>
-      <c r="G34" s="35"/>
-      <c r="H34" s="35"/>
-      <c r="I34" s="35"/>
-    </row>
-    <row r="35" spans="1:9" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A35" s="35"/>
-      <c r="B35" s="38">
-        <v>2</v>
-      </c>
-      <c r="C35" s="38" t="s">
-        <v>69</v>
-      </c>
-      <c r="D35" s="38"/>
-      <c r="E35" s="35"/>
-      <c r="F35" s="35"/>
-      <c r="G35" s="35"/>
-      <c r="H35" s="35"/>
-      <c r="I35" s="35"/>
-    </row>
-    <row r="36" spans="1:9" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A36" s="35"/>
-      <c r="B36" s="38">
-        <v>3</v>
-      </c>
-      <c r="C36" s="38" t="s">
-        <v>70</v>
-      </c>
-      <c r="D36" s="38"/>
-      <c r="E36" s="35"/>
-      <c r="F36" s="35"/>
-      <c r="G36" s="35"/>
-      <c r="H36" s="35"/>
-      <c r="I36" s="35"/>
-    </row>
-    <row r="37" spans="1:9" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A37" s="35"/>
-      <c r="B37" s="38"/>
-      <c r="C37" s="38"/>
-      <c r="D37" s="38"/>
-      <c r="E37" s="35"/>
-      <c r="F37" s="35"/>
-      <c r="G37" s="35"/>
-      <c r="H37" s="35"/>
-      <c r="I37" s="35"/>
-    </row>
-    <row r="38" spans="1:9" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A38" s="35"/>
-      <c r="B38" s="37" t="s">
-        <v>32</v>
-      </c>
-      <c r="C38" s="38"/>
-      <c r="D38" s="38"/>
-      <c r="E38" s="35"/>
-      <c r="F38" s="35"/>
-      <c r="G38" s="35"/>
-      <c r="H38" s="35"/>
-      <c r="I38" s="35"/>
-    </row>
-    <row r="39" spans="1:9" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A39" s="35"/>
-      <c r="B39" s="38">
-        <v>1</v>
-      </c>
-      <c r="C39" s="38" t="s">
-        <v>71</v>
-      </c>
-      <c r="D39" s="38"/>
-      <c r="E39" s="35"/>
-      <c r="F39" s="35"/>
-      <c r="G39" s="35"/>
-      <c r="H39" s="35"/>
-      <c r="I39" s="35"/>
-    </row>
-    <row r="40" spans="1:9" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A40" s="35"/>
-      <c r="B40" s="38">
-        <v>2</v>
-      </c>
-      <c r="C40" s="38" t="s">
-        <v>72</v>
-      </c>
-      <c r="D40" s="38"/>
-      <c r="E40" s="35"/>
-      <c r="F40" s="35"/>
-      <c r="G40" s="35"/>
-      <c r="H40" s="35"/>
-      <c r="I40" s="35"/>
-    </row>
-    <row r="41" spans="1:9" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A41" s="35"/>
-      <c r="B41" s="38">
-        <v>3</v>
-      </c>
-      <c r="C41" s="38" t="s">
-        <v>73</v>
-      </c>
-      <c r="D41" s="38"/>
-      <c r="E41" s="35"/>
-      <c r="F41" s="35"/>
-      <c r="G41" s="35"/>
-      <c r="H41" s="35"/>
-      <c r="I41" s="35"/>
-    </row>
-    <row r="42" spans="1:9" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A42" s="35"/>
-      <c r="B42" s="38">
-        <v>4</v>
-      </c>
-      <c r="C42" s="38" t="s">
-        <v>74</v>
-      </c>
-      <c r="D42" s="38"/>
-      <c r="E42" s="35"/>
-      <c r="F42" s="35"/>
-      <c r="G42" s="35"/>
-      <c r="H42" s="35"/>
-      <c r="I42" s="35"/>
-    </row>
-    <row r="43" spans="1:9" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A43" s="35"/>
-      <c r="B43" s="38">
-        <v>5</v>
-      </c>
-      <c r="C43" s="38" t="s">
-        <v>75</v>
-      </c>
-      <c r="D43" s="38"/>
-      <c r="E43" s="35"/>
-      <c r="F43" s="35"/>
-      <c r="G43" s="35"/>
-      <c r="H43" s="35"/>
-      <c r="I43" s="35"/>
-    </row>
-    <row r="44" spans="1:9" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A44" s="35"/>
-      <c r="B44" s="38">
-        <v>6</v>
-      </c>
-      <c r="C44" s="38" t="s">
-        <v>76</v>
-      </c>
-      <c r="D44" s="38"/>
-      <c r="E44" s="35"/>
-      <c r="F44" s="35"/>
-      <c r="G44" s="35"/>
-      <c r="H44" s="35"/>
-      <c r="I44" s="35"/>
-    </row>
-    <row r="45" spans="1:9" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A45" s="35"/>
-      <c r="B45" s="38"/>
-      <c r="C45" s="38"/>
-      <c r="D45" s="38"/>
-      <c r="E45" s="35"/>
-      <c r="F45" s="35"/>
-      <c r="G45" s="35"/>
-      <c r="H45" s="35"/>
-      <c r="I45" s="35"/>
-    </row>
-    <row r="46" spans="1:9" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A46" s="35"/>
-      <c r="B46" s="37" t="s">
-        <v>77</v>
-      </c>
-      <c r="C46" s="38"/>
-      <c r="D46" s="38"/>
-      <c r="E46" s="35"/>
-      <c r="F46" s="35"/>
-      <c r="G46" s="35"/>
-      <c r="H46" s="35"/>
-      <c r="I46" s="35"/>
-    </row>
-    <row r="47" spans="1:9" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A47" s="35"/>
-      <c r="B47" s="38">
-        <v>77</v>
-      </c>
-      <c r="C47" s="38" t="s">
-        <v>78</v>
-      </c>
-      <c r="D47" s="38"/>
-      <c r="E47" s="35"/>
-      <c r="F47" s="35"/>
-      <c r="G47" s="35"/>
-      <c r="H47" s="35"/>
-      <c r="I47" s="35"/>
-    </row>
-    <row r="48" spans="1:9" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A48" s="35"/>
-      <c r="B48" s="38">
-        <v>88</v>
-      </c>
-      <c r="C48" s="38" t="s">
-        <v>79</v>
-      </c>
-      <c r="D48" s="38"/>
-      <c r="E48" s="35"/>
-      <c r="F48" s="35"/>
-      <c r="G48" s="35"/>
-      <c r="H48" s="35"/>
-      <c r="I48" s="35"/>
-    </row>
-    <row r="49" spans="1:9" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A49" s="35"/>
-      <c r="B49" s="38">
-        <v>302</v>
-      </c>
-      <c r="C49" s="38" t="s">
-        <v>80</v>
-      </c>
-      <c r="D49" s="38"/>
-      <c r="E49" s="35"/>
-      <c r="F49" s="35"/>
-      <c r="G49" s="35"/>
-      <c r="H49" s="35"/>
-      <c r="I49" s="35"/>
-    </row>
-  </sheetData>
-  <mergeCells count="2">
-    <mergeCell ref="A3:I4"/>
-    <mergeCell ref="A5:I7"/>
-  </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>